<commit_message>
Adds and renames printed part quantities and updates BOM.
</commit_message>
<xml_diff>
--- a/BOM/voron_2_tall_bom.xlsx
+++ b/BOM/voron_2_tall_bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ppak/GitHub/Voron-2-Tall/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ppak/GitHub/Voron-2-Tall/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A886C59-0582-DB44-B89C-1921577900A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254316E7-914D-7043-9FA5-F4BA698ADC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="9380" windowWidth="33600" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LDO_bom" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="372">
   <si>
     <t>Category</t>
   </si>
@@ -877,12 +877,6 @@
     <t>Holes 10mm from each end</t>
   </si>
   <si>
-    <t>https://www.amazon.com/gp/product/B0C94YGTKX/ref=ox_sc_act_title_1?smid=A3E9XRLGZKR0KS&amp;th=1</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/gp/product/B0C94XJYH7/ref=ewc_pr_img_1?smid=A3E9XRLGZKR0KS&amp;th=1</t>
-  </si>
-  <si>
     <t>https://www.amazon.com/uxcell-Temperature-Multifunctional-Insulating-Transparent/dp/B0915QTF1G/ref=sr_1_5?crid=1TE27V508QIHN&amp;keywords=ptfe%2Btubing%2B1000mm%2B4mm%2BOD%2B3mm&amp;qid=1701900349&amp;s=industrial&amp;sprefix=ptfe%2Btubing%2B1000mm%2B4mm%2Bod%2B3mm%2Cindustrial%2C75&amp;sr=1-5&amp;th=1</t>
   </si>
   <si>
@@ -976,9 +970,6 @@
     <t>Orange Acrylic Sheet 36" x 24" x 1/8" (3mm)</t>
   </si>
   <si>
-    <t>Acrylic Sheet Clear 24" x 48" x 1/8"  (3mm)</t>
-  </si>
-  <si>
     <t>For General Printed Parts</t>
   </si>
   <si>
@@ -1010,6 +1001,156 @@
   </si>
   <si>
     <t>Self Source BOM (For Cost Comparison)</t>
+  </si>
+  <si>
+    <t>https://makerstock.com/products/orange-fluorescent-acrylic?variant=32575693357153</t>
+  </si>
+  <si>
+    <t>https://makerstock.com/products/orange-fluorescent-acrylic?variant=40860284026977</t>
+  </si>
+  <si>
+    <t>Orange Acrylic Sheet 24" x 48" x 1/8"  (3mm)</t>
+  </si>
+  <si>
+    <t>Protective coating over spray painted parts</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Krylon-I00500A00-12-Ounce-Triple-Aerosol/dp/B0CFXJGNMV/ref=sr_1_5?crid=1TJSAOK96C1KJ&amp;dib=eyJ2IjoiMSJ9.bD_eQuJFJ6yB5jINzIBwQ4gEhSZB6CVJHOYwBZMU95XFIeyPUwn92ww9yfBElzfJ822DDY37D_V2gtnVlKnaiUJZFxsHY7wqyR_jCS4RQk183xcO58brebRXQ93ELpAX9TReJR8qsUQERX6epb3iyUftw61lHe3-_bcAVeD652ou3rLsEihtNvRixIgqTQjXbqfk0ZDck8QuIJ1SsSLg1KtzfwLaFurm2itE-4XA-Y0XtP7AMERPOeXWw_1Ehu4igddft9ePFrxzZe89z5hY6K9LQiiNpP58iBPvE02zwVQ.qfLpFzIDMXBx808NxIveJoqucMsAi0DrfbnzwVESJak&amp;dib_tag=se&amp;keywords=clear%2Bcoat%2Bspray&amp;qid=1705719078&amp;sprefix=clear%2Bcoat%2Bspray%2Caps%2C112&amp;sr=8-5&amp;th=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B0C68HPHR2?psc=1&amp;ref=ppx_yo2ov_dt_b_product_details</t>
+  </si>
+  <si>
+    <t>BATIGE Micro HDMI Female &amp; Type C 3.0 Female Flush Mount</t>
+  </si>
+  <si>
+    <t>Optional port access to Raspberry Pi</t>
+  </si>
+  <si>
+    <t>Female 4P to Male 4P Motor Extension Wire</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B098J4MM3G?psc=1&amp;ref=ppx_yo2ov_dt_b_product_details</t>
+  </si>
+  <si>
+    <t>For A/B stepper and limit (Pack of 2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Krylon I00500A07 12-Ounce Triple Thick Clear Glaze Aerosol Spray,High-Gloss (Pack of 2) </t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Molex/43640-0201?qs=HlEFOAM0q6WaYhPmKKx%252BhQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Molex/43645-0200?qs=4XSMV6Twtb2TZ7elJDViLw%3D%3D</t>
+  </si>
+  <si>
+    <t>Stealthburner RGB Extender (Female)</t>
+  </si>
+  <si>
+    <t>Stealthburner RGB Extender (Male)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Headers &amp; Wire Housings PLUG FREE HNG 2P SINGLE ROW </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Headers &amp; Wire Housings RECEPTACLE 2 POS SINGLE ROW </t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/538-43020-1401</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Headers &amp; Wire Housings 14CKT PLUG HSG FREE HANGING DR </t>
+  </si>
+  <si>
+    <t>Stealthburner Extender (Female)</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/538-43031-0007</t>
+  </si>
+  <si>
+    <t>Headers &amp; Wire Housings MALE 20-24 AWG BULK tin</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Molex/43030-0007?qs=MuwpYaHj75276x2HQaDYIw%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Headers &amp; Wire Housings FEMALE TERM 20-24 </t>
+  </si>
+  <si>
+    <t>Crimps for female molex sockets</t>
+  </si>
+  <si>
+    <t>Crimps for male molex sockets</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/485-4559</t>
+  </si>
+  <si>
+    <t>Heat Shrink Tubing &amp; Sleeves Pre-Cut Multi-Colored Heat Shrink Pack</t>
+  </si>
+  <si>
+    <t>Various heatshrink for extenders</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/358-SC1131</t>
+  </si>
+  <si>
+    <t>FFC / FPC Jumper Cables Raspberry Pi 5 FPC Cables - Display, 200mm</t>
+  </si>
+  <si>
+    <t>Display Cable for Raspberry Pi 5</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/426-FIT0255</t>
+  </si>
+  <si>
+    <t>Educational Kits JST connector Kit (2.54mm)</t>
+  </si>
+  <si>
+    <t>JST connectors for trimming cables</t>
+  </si>
+  <si>
+    <t>Headers &amp; Wire Housings MicroFit Recep HSG DR 14Ckt GW BLK</t>
+  </si>
+  <si>
+    <t>Stealthburner Extender (Male)</t>
+  </si>
+  <si>
+    <t>Hook-up Wire 24AWG7/32 PTFE 100ft SPOOL WHT</t>
+  </si>
+  <si>
+    <t>PTFE wire stealhburner extenders</t>
+  </si>
+  <si>
+    <t>https://shop.pimoroni.com/products/nvme-base?variant=41219587178579</t>
+  </si>
+  <si>
+    <t>NVME Base for Raspberry Pi 5</t>
+  </si>
+  <si>
+    <t>Optional Raspberry Pi storage expansion</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>Remaining Subtotals</t>
+  </si>
+  <si>
+    <t>Overall</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Desired</t>
+  </si>
+  <si>
+    <t>Ordered</t>
+  </si>
+  <si>
+    <t>Paid</t>
   </si>
 </sst>
 </file>
@@ -1185,7 +1326,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1371,6 +1512,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1533,7 +1698,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
@@ -1541,6 +1706,12 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="8" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1897,29 +2068,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F651F1D0-7A81-0546-9600-A8B0A78885C7}">
-  <dimension ref="A1:K70"/>
+  <dimension ref="A1:K83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="49.33203125" customWidth="1"/>
+    <col min="1" max="1" width="57.5" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
     <col min="3" max="3" width="34.33203125" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" customWidth="1"/>
     <col min="5" max="5" width="11.5" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="8" width="11" customWidth="1"/>
-    <col min="9" max="9" width="12.5" customWidth="1"/>
-    <col min="10" max="10" width="16.1640625" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" customWidth="1"/>
     <col min="11" max="11" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1932,6 +2104,16 @@
         <v>262</v>
       </c>
     </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F4" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="G4" s="9"/>
+      <c r="I4" s="10" t="s">
+        <v>366</v>
+      </c>
+      <c r="J4" s="11"/>
+    </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
@@ -1943,25 +2125,25 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>200</v>
+        <v>365</v>
       </c>
       <c r="E5" t="s">
         <v>114</v>
       </c>
-      <c r="F5" t="s">
-        <v>252</v>
-      </c>
-      <c r="G5" t="s">
-        <v>253</v>
+      <c r="F5" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>370</v>
       </c>
       <c r="H5" t="s">
-        <v>199</v>
-      </c>
-      <c r="I5" t="s">
-        <v>198</v>
-      </c>
-      <c r="J5" t="s">
-        <v>223</v>
+        <v>371</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>365</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>367</v>
       </c>
       <c r="K5" t="s">
         <v>115</v>
@@ -1969,13 +2151,13 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
@@ -1983,26 +2165,26 @@
       <c r="E6" s="1">
         <v>1449</v>
       </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
+      <c r="F6" s="7">
+        <v>1</v>
+      </c>
+      <c r="G6" s="7">
         <v>0</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" ref="H6:H9" si="0">IF(NOT(D6), E6*F6, E6*0)</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="1">
-        <f t="shared" ref="I6:I9" si="1">IF(D6, E6*F6, E6*0)</f>
+        <f>G6*E6</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="12">
+        <f t="shared" ref="I6:I9" si="0">IF(D6, E6*F6, E6*0)</f>
         <v>1449</v>
       </c>
-      <c r="J6" s="1">
-        <f t="shared" ref="J6:J9" si="2">(F6-G6)*E6</f>
+      <c r="J6" s="12">
+        <f t="shared" ref="J6:J9" si="1">(F6-G6)*E6</f>
         <v>1449</v>
       </c>
       <c r="K6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -2021,37 +2203,37 @@
       <c r="E7" s="1">
         <v>12.88</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="7">
         <v>2</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="7">
         <v>0</v>
       </c>
       <c r="H7" s="1">
+        <f t="shared" ref="H7:H31" si="2">G7*E7</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I7" s="1">
+        <v>25.76</v>
+      </c>
+      <c r="J7" s="12">
         <f t="shared" si="1"/>
         <v>25.76</v>
       </c>
-      <c r="J7" s="1">
-        <f t="shared" si="2"/>
-        <v>25.76</v>
-      </c>
       <c r="K7" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D8" t="b">
         <v>1</v>
@@ -2059,22 +2241,22 @@
       <c r="E8" s="1">
         <v>30.91</v>
       </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
+      <c r="F8" s="7">
+        <v>1</v>
+      </c>
+      <c r="G8" s="7">
         <v>0</v>
       </c>
       <c r="H8" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I8" s="1">
+        <v>30.91</v>
+      </c>
+      <c r="J8" s="12">
         <f t="shared" si="1"/>
-        <v>30.91</v>
-      </c>
-      <c r="J8" s="1">
-        <f t="shared" si="2"/>
         <v>30.91</v>
       </c>
       <c r="K8" s="2" t="s">
@@ -2094,22 +2276,22 @@
       <c r="E9" s="3">
         <v>66</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="7">
         <v>4</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="7">
         <v>0</v>
       </c>
       <c r="H9" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I9" s="1">
+        <v>264</v>
+      </c>
+      <c r="J9" s="12">
         <f t="shared" si="1"/>
-        <v>264</v>
-      </c>
-      <c r="J9" s="1">
-        <f t="shared" si="2"/>
         <v>264</v>
       </c>
       <c r="K9" s="2" t="s">
@@ -2132,22 +2314,22 @@
       <c r="E10" s="1">
         <v>25.97</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="7">
         <v>4</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="7">
         <v>0</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" ref="H10:H16" si="3">IF(NOT(D10), E10*F10, E10*0)</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="1">
-        <f t="shared" ref="I10:I17" si="4">IF(D10, E10*F10, E10*0)</f>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="12">
+        <f t="shared" ref="I10:I31" si="3">IF(D10, E10*F10, E10*0)</f>
         <v>103.88</v>
       </c>
-      <c r="J10" s="1">
-        <f t="shared" ref="J10" si="5">(F10-G10)*E10</f>
+      <c r="J10" s="12">
+        <f t="shared" ref="J10" si="4">(F10-G10)*E10</f>
         <v>103.88</v>
       </c>
       <c r="K10" t="s">
@@ -2162,7 +2344,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
@@ -2170,37 +2352,37 @@
       <c r="E11" s="1">
         <v>7.99</v>
       </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
+      <c r="F11" s="7">
+        <v>1</v>
+      </c>
+      <c r="G11" s="7">
         <v>0</v>
       </c>
       <c r="H11" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I11" s="1">
-        <f t="shared" si="4"/>
         <v>7.99</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="12">
         <f>(F11-G11)*E11</f>
         <v>7.99</v>
       </c>
       <c r="K11" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D12" t="b">
         <v>1</v>
@@ -2208,26 +2390,26 @@
       <c r="E12" s="1">
         <v>89.54</v>
       </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
+      <c r="F12" s="7">
+        <v>1</v>
+      </c>
+      <c r="G12" s="7">
         <v>0</v>
       </c>
       <c r="H12" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="1">
-        <f t="shared" si="4"/>
         <v>89.54</v>
       </c>
-      <c r="J12" s="1">
-        <f t="shared" ref="J12:J14" si="6">(F12-G12)*E12</f>
+      <c r="J12" s="12">
+        <f t="shared" ref="J12:J14" si="5">(F12-G12)*E12</f>
         <v>89.54</v>
       </c>
       <c r="K12" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -2238,7 +2420,7 @@
         <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
@@ -2246,37 +2428,37 @@
       <c r="E13" s="1">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="7">
         <v>100</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="7">
         <v>0</v>
       </c>
       <c r="H13" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="1">
-        <f t="shared" si="4"/>
         <v>8.3000000000000007</v>
       </c>
-      <c r="J13" s="1">
-        <f t="shared" si="6"/>
+      <c r="J13" s="12">
+        <f t="shared" si="5"/>
         <v>8.3000000000000007</v>
       </c>
       <c r="K13" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D14" t="b">
         <v>1</v>
@@ -2284,26 +2466,26 @@
       <c r="E14" s="1">
         <v>1.02</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="7">
         <v>2</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="7">
         <v>0</v>
       </c>
       <c r="H14" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I14" s="1">
-        <f t="shared" si="4"/>
         <v>2.04</v>
       </c>
-      <c r="J14" s="1">
-        <f t="shared" si="6"/>
+      <c r="J14" s="12">
+        <f t="shared" si="5"/>
         <v>2.04</v>
       </c>
       <c r="K14" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -2322,22 +2504,22 @@
       <c r="E15" s="1">
         <v>46.44</v>
       </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
+      <c r="F15" s="7">
+        <v>1</v>
+      </c>
+      <c r="G15" s="7">
         <v>0</v>
       </c>
       <c r="H15" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="1">
-        <f t="shared" si="4"/>
         <v>46.44</v>
       </c>
-      <c r="J15" s="1">
-        <f t="shared" ref="J15:J17" si="7">(F15-G15)*E15</f>
+      <c r="J15" s="12">
+        <f t="shared" ref="J15:J31" si="6">(F15-G15)*E15</f>
         <v>46.44</v>
       </c>
       <c r="K15" s="2" t="s">
@@ -2357,22 +2539,22 @@
       <c r="E16" s="1">
         <v>6.12</v>
       </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
+      <c r="F16" s="7">
+        <v>1</v>
+      </c>
+      <c r="G16" s="7">
         <v>0</v>
       </c>
       <c r="H16" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="1">
-        <f t="shared" si="4"/>
         <v>6.12</v>
       </c>
-      <c r="J16" s="1">
-        <f t="shared" si="7"/>
+      <c r="J16" s="12">
+        <f t="shared" si="6"/>
         <v>6.12</v>
       </c>
       <c r="K16" s="2" t="s">
@@ -2381,13 +2563,13 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D17" t="b">
         <v>1</v>
@@ -2395,22 +2577,22 @@
       <c r="E17" s="1">
         <v>139.80000000000001</v>
       </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
+      <c r="F17" s="7">
+        <v>1</v>
+      </c>
+      <c r="G17" s="7">
         <v>0</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" ref="H17" si="8">IF(NOT(D17), E17*F17, E17*0)</f>
-        <v>0</v>
-      </c>
-      <c r="I17" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="12">
+        <f t="shared" si="3"/>
         <v>139.80000000000001</v>
       </c>
-      <c r="J17" s="1">
-        <f t="shared" si="7"/>
+      <c r="J17" s="12">
+        <f t="shared" si="6"/>
         <v>139.80000000000001</v>
       </c>
       <c r="K17" s="2" t="s">
@@ -2419,35 +2601,534 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="E18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E19" s="1"/>
+      <c r="A19" t="s">
+        <v>330</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>332</v>
+      </c>
+      <c r="D19" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
+        <v>12.99</v>
+      </c>
+      <c r="F19" s="7">
+        <v>2</v>
+      </c>
+      <c r="G19" s="7">
+        <v>0</v>
+      </c>
       <c r="H19" s="1">
-        <f>SUM(H6:H18)</f>
-        <v>0</v>
-      </c>
-      <c r="I19" s="1">
-        <f>SUM(I6:I18)</f>
-        <v>2173.7800000000002</v>
-      </c>
-      <c r="J19" s="1">
-        <f>SUM(J6:J18)</f>
-        <v>2173.7800000000002</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="12">
+        <f t="shared" si="3"/>
+        <v>25.98</v>
+      </c>
+      <c r="J19" s="12">
+        <f t="shared" si="6"/>
+        <v>25.98</v>
+      </c>
+      <c r="K19" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>328</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>329</v>
+      </c>
+      <c r="D20" t="b">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <v>15.99</v>
+      </c>
+      <c r="F20" s="7">
+        <v>1</v>
+      </c>
+      <c r="G20" s="7">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="12">
+        <f t="shared" si="6"/>
+        <v>15.99</v>
+      </c>
+      <c r="K20" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>338</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>336</v>
+      </c>
+      <c r="D21" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="F21" s="7">
+        <v>2</v>
+      </c>
+      <c r="G21" s="7">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="12">
+        <f t="shared" si="3"/>
+        <v>0.76</v>
+      </c>
+      <c r="J21" s="12">
+        <f t="shared" si="6"/>
+        <v>0.76</v>
+      </c>
+      <c r="K21" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>339</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>337</v>
+      </c>
+      <c r="D22" t="b">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="F22" s="7">
+        <v>2</v>
+      </c>
+      <c r="G22" s="7">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="12">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
+      <c r="J22" s="12">
+        <f t="shared" si="6"/>
+        <v>0.8</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>341</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>342</v>
+      </c>
+      <c r="D23" t="b">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="F23" s="7">
+        <v>2</v>
+      </c>
+      <c r="G23" s="7">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="12">
+        <f t="shared" si="3"/>
+        <v>1.72</v>
+      </c>
+      <c r="J23" s="12">
+        <f t="shared" si="6"/>
+        <v>1.72</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>358</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>359</v>
+      </c>
+      <c r="D24" t="b">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1.02</v>
+      </c>
+      <c r="F24" s="7">
+        <v>2</v>
+      </c>
+      <c r="G24" s="7">
+        <v>0</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="12">
+        <f t="shared" si="3"/>
+        <v>2.04</v>
+      </c>
+      <c r="J24" s="12">
+        <f t="shared" si="6"/>
+        <v>2.04</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>344</v>
+      </c>
+      <c r="B25">
+        <v>16</v>
+      </c>
+      <c r="C25" t="s">
+        <v>347</v>
+      </c>
+      <c r="D25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.122</v>
+      </c>
+      <c r="F25" s="7">
+        <v>100</v>
+      </c>
+      <c r="G25" s="7">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="12">
+        <f t="shared" si="3"/>
+        <v>12.2</v>
+      </c>
+      <c r="J25" s="12">
+        <f t="shared" si="6"/>
+        <v>12.2</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>346</v>
+      </c>
+      <c r="B26">
+        <v>16</v>
+      </c>
+      <c r="C26" t="s">
+        <v>348</v>
+      </c>
+      <c r="D26" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.114</v>
+      </c>
+      <c r="F26" s="7">
+        <v>100</v>
+      </c>
+      <c r="G26" s="7">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="12">
+        <f t="shared" si="3"/>
+        <v>11.4</v>
+      </c>
+      <c r="J26" s="12">
+        <f t="shared" si="6"/>
+        <v>11.4</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>350</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>351</v>
+      </c>
+      <c r="D27" t="b">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="F27" s="7">
+        <v>1</v>
+      </c>
+      <c r="G27" s="7">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="12">
+        <f t="shared" si="3"/>
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="J27" s="12">
+        <f t="shared" si="6"/>
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>353</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>354</v>
+      </c>
+      <c r="D28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
+      <c r="F28" s="7">
+        <v>1</v>
+      </c>
+      <c r="G28" s="7">
+        <v>0</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="12">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>356</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>357</v>
+      </c>
+      <c r="D29" t="b">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1">
+        <v>8.9</v>
+      </c>
+      <c r="F29" s="7">
+        <v>1</v>
+      </c>
+      <c r="G29" s="7">
+        <v>0</v>
+      </c>
+      <c r="H29" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="12">
+        <f t="shared" si="3"/>
+        <v>8.9</v>
+      </c>
+      <c r="J29" s="12">
+        <f t="shared" si="6"/>
+        <v>8.9</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>360</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>361</v>
+      </c>
+      <c r="D30" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" s="1">
+        <v>89.54</v>
+      </c>
+      <c r="F30" s="7">
+        <v>1</v>
+      </c>
+      <c r="G30" s="7">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I30" s="12">
+        <f t="shared" si="3"/>
+        <v>89.54</v>
+      </c>
+      <c r="J30" s="12">
+        <f t="shared" si="6"/>
+        <v>89.54</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>363</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>364</v>
+      </c>
+      <c r="D31" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <v>14.36</v>
+      </c>
+      <c r="F31" s="7">
+        <v>1</v>
+      </c>
+      <c r="G31" s="7">
+        <v>0</v>
+      </c>
+      <c r="H31" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I31" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J31" s="12">
+        <f t="shared" si="6"/>
+        <v>14.36</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E32" s="1"/>
+      <c r="H32" s="1">
+        <f>SUM(H6:H31)</f>
+        <v>0</v>
+      </c>
+      <c r="I32" s="1">
+        <f>SUM(I6:I31)</f>
+        <v>2337.0700000000002</v>
+      </c>
+      <c r="J32" s="1">
+        <f>SUM(J6:J31)</f>
+        <v>2368.42</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2458,6 +3139,7 @@
     <hyperlink ref="K17" r:id="rId3" xr:uid="{933BC923-64A5-364D-B1D1-AA0CD0F86FE7}"/>
     <hyperlink ref="K16" r:id="rId4" xr:uid="{040C449F-BD13-3A40-A3CF-B6CEB04C54CC}"/>
     <hyperlink ref="K15" r:id="rId5" xr:uid="{1BE03111-1688-3547-8700-06A03759C772}"/>
+    <hyperlink ref="K22" r:id="rId6" xr:uid="{54E046B7-4373-0C4C-B1FF-977F5691AE73}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2465,9 +3147,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4686087C-B58C-7A42-AAAC-3D022FB0521D}">
-  <dimension ref="A1:K66"/>
+  <dimension ref="A1:K67"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2486,7 +3170,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -2536,13 +3220,13 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
@@ -2554,33 +3238,33 @@
         <v>2</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" ref="H6:H7" si="0">IF(NOT(D6), E6*F6, E6*0)</f>
         <v>0</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" ref="I6:I13" si="1">IF(D6, E6*F6, E6*0)</f>
+        <f t="shared" ref="I6:I14" si="1">IF(D6, E6*F6, E6*0)</f>
         <v>14.48</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" ref="J6:J14" si="2">(F6-G6)*E6</f>
-        <v>0</v>
+        <f t="shared" ref="J6:J15" si="2">(F6-G6)*E6</f>
+        <v>14.48</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D7" t="b">
         <v>1</v>
@@ -2592,7 +3276,7 @@
         <v>2</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="0"/>
@@ -2604,30 +3288,30 @@
       </c>
       <c r="J7" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15.4</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D8" t="b">
         <v>1</v>
       </c>
       <c r="E8" s="1">
-        <v>39.950000000000003</v>
+        <v>24.95</v>
       </c>
       <c r="F8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -2637,19 +3321,19 @@
       </c>
       <c r="I8" s="1">
         <f t="shared" si="1"/>
-        <v>119.85000000000001</v>
+        <v>49.9</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="2"/>
-        <v>119.85000000000001</v>
+        <v>49.9</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>280</v>
+        <v>322</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E9" s="1"/>
       <c r="H9" s="1"/>
@@ -2659,19 +3343,19 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>313</v>
+        <v>324</v>
       </c>
       <c r="B10">
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
       </c>
       <c r="E10" s="1">
-        <v>52.95</v>
+        <v>49.95</v>
       </c>
       <c r="F10">
         <v>4</v>
@@ -2680,38 +3364,35 @@
         <v>0</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" ref="H10:H13" si="3">IF(NOT(D10), E10*F10, E10*0)</f>
+        <f t="shared" ref="H10:H14" si="3">IF(NOT(D10), E10*F10, E10*0)</f>
         <v>0</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="1"/>
-        <v>211.8</v>
+        <v>199.8</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="2"/>
-        <v>211.8</v>
+        <v>199.8</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>281</v>
+        <v>323</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
-        <v>311</v>
-      </c>
-      <c r="D11" t="b">
-        <v>1</v>
+        <v>309</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D12" t="b">
         <v>1</v>
@@ -2738,18 +3419,18 @@
         <v>39.979999999999997</v>
       </c>
       <c r="K12" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
@@ -2776,68 +3457,106 @@
         <v>21.99</v>
       </c>
       <c r="K13" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>292</v>
+        <v>333</v>
       </c>
       <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>325</v>
+      </c>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>12.94</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="1"/>
+        <v>25.88</v>
+      </c>
+      <c r="J14" s="1">
+        <f t="shared" si="2"/>
+        <v>25.88</v>
+      </c>
+      <c r="K14" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>290</v>
+      </c>
+      <c r="B15">
         <v>8</v>
       </c>
-      <c r="C14" t="s">
-        <v>316</v>
-      </c>
-      <c r="D14" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1">
+      <c r="C15" t="s">
+        <v>313</v>
+      </c>
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
         <v>6.04</v>
       </c>
-      <c r="F14">
+      <c r="F15">
         <v>8</v>
       </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14" s="1">
-        <f t="shared" ref="H14" si="4">IF(NOT(D14), E14*F14, E14*0)</f>
-        <v>0</v>
-      </c>
-      <c r="I14" s="1">
-        <f t="shared" ref="I14" si="5">IF(D14, E14*F14, E14*0)</f>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" ref="H15" si="4">IF(NOT(D15), E15*F15, E15*0)</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" ref="I15" si="5">IF(D15, E15*F15, E15*0)</f>
         <v>48.32</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J15" s="1">
         <f t="shared" si="2"/>
         <v>48.32</v>
       </c>
-      <c r="K14" s="2" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H15" s="1">
+      <c r="K15" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H16" s="1">
         <f>SUM(H6:H10)</f>
         <v>0</v>
       </c>
-      <c r="I15" s="1">
-        <f>SUM(I6:I14)</f>
-        <v>471.82000000000005</v>
-      </c>
-      <c r="J15" s="1">
-        <f>SUM(J6:J14)</f>
-        <v>441.94000000000005</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+      <c r="I16" s="1">
+        <f>SUM(I6:I15)</f>
+        <v>415.75000000000006</v>
+      </c>
+      <c r="J16" s="1">
+        <f>SUM(J6:J15)</f>
+        <v>415.75000000000006</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2845,7 +3564,7 @@
   <hyperlinks>
     <hyperlink ref="K10" r:id="rId1" xr:uid="{D015C5EB-6B16-0744-8964-924D048D7799}"/>
     <hyperlink ref="K8" r:id="rId2" xr:uid="{87546791-3990-2846-B60F-64D77FF64AB4}"/>
-    <hyperlink ref="K14" r:id="rId3" xr:uid="{8FEB2D40-243D-EB40-9049-84074FF0142B}"/>
+    <hyperlink ref="K15" r:id="rId3" xr:uid="{8FEB2D40-243D-EB40-9049-84074FF0142B}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2875,7 +3594,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="26" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -5939,7 +6658,7 @@
         <v>1</v>
       </c>
       <c r="D89" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E89" t="b">
         <v>1</v>
@@ -5966,7 +6685,7 @@
         <v>7.99</v>
       </c>
       <c r="L89" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.2">
@@ -5977,7 +6696,7 @@
         <v>1</v>
       </c>
       <c r="D90" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E90" t="b">
         <v>1</v>
@@ -6004,7 +6723,7 @@
         <v>8.99</v>
       </c>
       <c r="L90" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.2">
@@ -6317,13 +7036,13 @@
     </row>
     <row r="101" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C101">
         <v>1</v>
       </c>
       <c r="D101" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E101" t="b">
         <v>1</v>
@@ -6350,7 +7069,7 @@
         <v>89.54</v>
       </c>
       <c r="L101" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="102" spans="2:12" x14ac:dyDescent="0.2">
@@ -6361,7 +7080,7 @@
         <v>28</v>
       </c>
       <c r="D102" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E102" t="b">
         <v>1</v>
@@ -6388,18 +7107,18 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="L102" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="103" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C103">
         <v>2</v>
       </c>
       <c r="D103" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E103" t="b">
         <v>1</v>
@@ -6426,7 +7145,7 @@
         <v>2.04</v>
       </c>
       <c r="L103" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="104" spans="2:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Adds `.cdr` files for panels and reorganizes related files.
</commit_message>
<xml_diff>
--- a/BOM/voron_2_tall_bom.xlsx
+++ b/BOM/voron_2_tall_bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ppak/GitHub/Voron-2-Tall/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254316E7-914D-7043-9FA5-F4BA698ADC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D734DE-EC3F-E14C-9C78-D13B89E73AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="9380" windowWidth="33600" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="33600" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LDO_bom" sheetId="2" r:id="rId1"/>
@@ -3575,7 +3575,7 @@
   <dimension ref="A1:L130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="L74" sqref="L74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6162,7 +6162,7 @@
         <f t="shared" si="7"/>
         <v>11.96</v>
       </c>
-      <c r="L74" t="s">
+      <c r="L74" s="2" t="s">
         <v>185</v>
       </c>
     </row>
@@ -8083,6 +8083,7 @@
     <hyperlink ref="L119" r:id="rId7" xr:uid="{AEBA3306-F4D8-AE42-9060-914CB8AFFD5A}"/>
     <hyperlink ref="L120" r:id="rId8" xr:uid="{AD2D870A-912A-784D-A7EF-5A36FCA6A342}"/>
     <hyperlink ref="L104" r:id="rId9" xr:uid="{4BDDBBBB-A24C-1E48-BA79-613613746B29}"/>
+    <hyperlink ref="L74" r:id="rId10" xr:uid="{1F2C7E8B-FA39-5241-82D7-118454574223}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updates `BOM` with more parts, adds print ready panels, and used `.stl`s.
</commit_message>
<xml_diff>
--- a/BOM/voron_2_tall_bom.xlsx
+++ b/BOM/voron_2_tall_bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ppak/GitHub/Voron-2-Tall/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D734DE-EC3F-E14C-9C78-D13B89E73AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986CA084-DA29-4F42-AC94-7EBADB5EBD72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="33600" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LDO_bom" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="376">
   <si>
     <t>Category</t>
   </si>
@@ -1151,6 +1151,18 @@
   </si>
   <si>
     <t>Paid</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07B8CK8L9/ref=ppx_yo_dt_b_asin_title_o00_s00?ie=UTF8&amp;th=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B09B2CGW12?psc=1&amp;ref=ppx_yo2ov_dt_b_product_details</t>
+  </si>
+  <si>
+    <t>Pack of 100 (silver color to match theme)</t>
+  </si>
+  <si>
+    <t>M3-0.5 x 8mm Socket Head Cap Screws Bolts</t>
   </si>
 </sst>
 </file>
@@ -2068,10 +2080,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F651F1D0-7A81-0546-9600-A8B0A78885C7}">
-  <dimension ref="A1:K83"/>
+  <dimension ref="A1:K84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2176,11 +2188,11 @@
         <v>0</v>
       </c>
       <c r="I6" s="12">
-        <f t="shared" ref="I6:I9" si="0">IF(D6, E6*F6, E6*0)</f>
+        <f t="shared" ref="I6:I10" si="0">IF(D6, E6*F6, E6*0)</f>
         <v>1449</v>
       </c>
       <c r="J6" s="12">
-        <f t="shared" ref="J6:J9" si="1">(F6-G6)*E6</f>
+        <f t="shared" ref="J6:J10" si="1">(F6-G6)*E6</f>
         <v>1449</v>
       </c>
       <c r="K6" t="s">
@@ -2189,95 +2201,97 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>375</v>
       </c>
       <c r="B7">
-        <v>163</v>
+        <v>100</v>
       </c>
       <c r="C7" t="s">
-        <v>137</v>
+        <v>374</v>
       </c>
       <c r="D7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1">
-        <v>12.88</v>
+        <v>5.99</v>
       </c>
       <c r="F7" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7" s="7">
         <v>0</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" ref="H7:H31" si="2">G7*E7</f>
         <v>0</v>
       </c>
       <c r="I7" s="12">
         <f t="shared" si="0"/>
-        <v>25.76</v>
+        <v>0</v>
       </c>
       <c r="J7" s="12">
         <f t="shared" si="1"/>
-        <v>25.76</v>
+        <v>5.99</v>
       </c>
       <c r="K7" t="s">
-        <v>138</v>
+        <v>373</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>302</v>
+        <v>23</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>163</v>
       </c>
       <c r="C8" t="s">
-        <v>303</v>
+        <v>137</v>
       </c>
       <c r="D8" t="b">
         <v>1</v>
       </c>
       <c r="E8" s="1">
-        <v>30.91</v>
+        <v>12.88</v>
       </c>
       <c r="F8" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" s="7">
         <v>0</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="H8:H32" si="2">G8*E8</f>
         <v>0</v>
       </c>
       <c r="I8" s="12">
         <f t="shared" si="0"/>
-        <v>30.91</v>
+        <v>25.76</v>
       </c>
       <c r="J8" s="12">
         <f t="shared" si="1"/>
-        <v>30.91</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>145</v>
+        <v>25.76</v>
+      </c>
+      <c r="K8" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>267</v>
+        <v>302</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>303</v>
       </c>
       <c r="D9" t="b">
         <v>1</v>
       </c>
-      <c r="E9" s="3">
-        <v>66</v>
+      <c r="E9" s="1">
+        <v>30.91</v>
       </c>
       <c r="F9" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G9" s="7">
         <v>0</v>
@@ -2288,31 +2302,28 @@
       </c>
       <c r="I9" s="12">
         <f t="shared" si="0"/>
-        <v>264</v>
+        <v>30.91</v>
       </c>
       <c r="J9" s="12">
         <f t="shared" si="1"/>
-        <v>264</v>
+        <v>30.91</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>268</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="B10">
         <v>4</v>
       </c>
-      <c r="C10" t="s">
-        <v>279</v>
-      </c>
       <c r="D10" t="b">
         <v>1</v>
       </c>
-      <c r="E10" s="1">
-        <v>25.97</v>
+      <c r="E10" s="3">
+        <v>66</v>
       </c>
       <c r="F10" s="7">
         <v>4</v>
@@ -2325,35 +2336,35 @@
         <v>0</v>
       </c>
       <c r="I10" s="12">
-        <f t="shared" ref="I10:I31" si="3">IF(D10, E10*F10, E10*0)</f>
-        <v>103.88</v>
+        <f t="shared" si="0"/>
+        <v>264</v>
       </c>
       <c r="J10" s="12">
-        <f t="shared" ref="J10" si="4">(F10-G10)*E10</f>
-        <v>103.88</v>
-      </c>
-      <c r="K10" t="s">
-        <v>278</v>
+        <f t="shared" si="1"/>
+        <v>264</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>274</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
       </c>
       <c r="E11" s="1">
-        <v>7.99</v>
+        <v>25.97</v>
       </c>
       <c r="F11" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G11" s="7">
         <v>0</v>
@@ -2363,32 +2374,32 @@
         <v>0</v>
       </c>
       <c r="I11" s="12">
-        <f t="shared" si="3"/>
-        <v>7.99</v>
+        <f t="shared" ref="I11:I32" si="3">IF(D11, E11*F11, E11*0)</f>
+        <v>103.88</v>
       </c>
       <c r="J11" s="12">
-        <f>(F11-G11)*E11</f>
-        <v>7.99</v>
+        <f t="shared" ref="J11" si="4">(F11-G11)*E11</f>
+        <v>103.88</v>
       </c>
       <c r="K11" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>296</v>
+        <v>78</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>297</v>
+        <v>281</v>
       </c>
       <c r="D12" t="b">
         <v>1</v>
       </c>
       <c r="E12" s="1">
-        <v>89.54</v>
+        <v>8.99</v>
       </c>
       <c r="F12" s="7">
         <v>1</v>
@@ -2402,34 +2413,34 @@
       </c>
       <c r="I12" s="12">
         <f t="shared" si="3"/>
-        <v>89.54</v>
+        <v>8.99</v>
       </c>
       <c r="J12" s="12">
-        <f t="shared" ref="J12:J14" si="5">(F12-G12)*E12</f>
-        <v>89.54</v>
+        <f>(F12-G12)*E12</f>
+        <v>8.99</v>
       </c>
       <c r="K12" t="s">
-        <v>298</v>
+        <v>372</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>296</v>
       </c>
       <c r="B13">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
       </c>
       <c r="E13" s="1">
-        <v>8.3000000000000004E-2</v>
+        <v>89.54</v>
       </c>
       <c r="F13" s="7">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="G13" s="7">
         <v>0</v>
@@ -2440,574 +2451,574 @@
       </c>
       <c r="I13" s="12">
         <f t="shared" si="3"/>
+        <v>89.54</v>
+      </c>
+      <c r="J13" s="12">
+        <f t="shared" ref="J13:J15" si="5">(F13-G13)*E13</f>
+        <v>89.54</v>
+      </c>
+      <c r="K13" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>294</v>
+      </c>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="F14" s="7">
+        <v>100</v>
+      </c>
+      <c r="G14" s="7">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="12">
+        <f t="shared" si="3"/>
         <v>8.3000000000000007</v>
       </c>
-      <c r="J13" s="12">
+      <c r="J14" s="12">
         <f t="shared" si="5"/>
         <v>8.3000000000000007</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K14" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>292</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>2</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>293</v>
       </c>
-      <c r="D14" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1">
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
         <v>1.02</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F15" s="7">
         <v>2</v>
       </c>
-      <c r="G14" s="7">
-        <v>0</v>
-      </c>
-      <c r="H14" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I14" s="12">
+      <c r="G15" s="7">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="12">
         <f t="shared" si="3"/>
         <v>2.04</v>
       </c>
-      <c r="J14" s="12">
+      <c r="J15" s="12">
         <f t="shared" si="5"/>
         <v>2.04</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K15" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>276</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
         <v>277</v>
       </c>
-      <c r="D15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1">
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
         <v>46.44</v>
       </c>
-      <c r="F15" s="7">
-        <v>1</v>
-      </c>
-      <c r="G15" s="7">
-        <v>0</v>
-      </c>
-      <c r="H15" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="12">
+      <c r="F16" s="7">
+        <v>1</v>
+      </c>
+      <c r="G16" s="7">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="12">
         <f t="shared" si="3"/>
         <v>46.44</v>
       </c>
-      <c r="J15" s="12">
-        <f t="shared" ref="J15:J31" si="6">(F15-G15)*E15</f>
+      <c r="J16" s="12">
+        <f t="shared" ref="J16:J32" si="6">(F16-G16)*E16</f>
         <v>46.44</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="K16" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>101</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="D16" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" s="1">
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
         <v>6.12</v>
       </c>
-      <c r="F16" s="7">
-        <v>1</v>
-      </c>
-      <c r="G16" s="7">
-        <v>0</v>
-      </c>
-      <c r="H16" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="12">
+      <c r="F17" s="7">
+        <v>1</v>
+      </c>
+      <c r="G17" s="7">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="12">
         <f t="shared" si="3"/>
         <v>6.12</v>
       </c>
-      <c r="J16" s="12">
+      <c r="J17" s="12">
         <f t="shared" si="6"/>
         <v>6.12</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="K17" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>320</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
         <v>317</v>
       </c>
-      <c r="D17" t="b">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1">
+      <c r="D18" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
         <v>139.80000000000001</v>
       </c>
-      <c r="F17" s="7">
-        <v>1</v>
-      </c>
-      <c r="G17" s="7">
-        <v>0</v>
-      </c>
-      <c r="H17" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="12">
+      <c r="F18" s="7">
+        <v>1</v>
+      </c>
+      <c r="G18" s="7">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="12">
         <f t="shared" si="3"/>
         <v>139.80000000000001</v>
       </c>
-      <c r="J17" s="12">
+      <c r="J18" s="12">
         <f t="shared" si="6"/>
         <v>139.80000000000001</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="K18" s="2" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C18" t="s">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
         <v>318</v>
       </c>
-      <c r="E18" s="1"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="E19" s="1"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>330</v>
       </c>
-      <c r="B19">
+      <c r="B20">
         <v>2</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>332</v>
       </c>
-      <c r="D19" t="b">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1">
+      <c r="D20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
         <v>12.99</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F20" s="7">
         <v>2</v>
       </c>
-      <c r="G19" s="7">
-        <v>0</v>
-      </c>
-      <c r="H19" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I19" s="12">
+      <c r="G20" s="7">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="12">
         <f t="shared" si="3"/>
         <v>25.98</v>
       </c>
-      <c r="J19" s="12">
+      <c r="J20" s="12">
         <f t="shared" si="6"/>
         <v>25.98</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K20" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>328</v>
       </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
         <v>329</v>
       </c>
-      <c r="D20" t="b">
-        <v>0</v>
-      </c>
-      <c r="E20" s="1">
+      <c r="D21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
         <v>15.99</v>
       </c>
-      <c r="F20" s="7">
-        <v>1</v>
-      </c>
-      <c r="G20" s="7">
-        <v>0</v>
-      </c>
-      <c r="H20" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I20" s="12">
+      <c r="F21" s="7">
+        <v>1</v>
+      </c>
+      <c r="G21" s="7">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="12">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="J20" s="12">
+      <c r="J21" s="12">
         <f t="shared" si="6"/>
         <v>15.99</v>
       </c>
-      <c r="K20" t="s">
+      <c r="K21" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>338</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
         <v>336</v>
       </c>
-      <c r="D21" t="b">
-        <v>1</v>
-      </c>
-      <c r="E21" s="1">
+      <c r="D22" t="b">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
         <v>0.38</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F22" s="7">
         <v>2</v>
       </c>
-      <c r="G21" s="7">
-        <v>0</v>
-      </c>
-      <c r="H21" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I21" s="12">
+      <c r="G22" s="7">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="12">
         <f t="shared" si="3"/>
         <v>0.76</v>
       </c>
-      <c r="J21" s="12">
+      <c r="J22" s="12">
         <f t="shared" si="6"/>
         <v>0.76</v>
       </c>
-      <c r="K21" t="s">
+      <c r="K22" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>339</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
         <v>337</v>
       </c>
-      <c r="D22" t="b">
-        <v>1</v>
-      </c>
-      <c r="E22" s="1">
+      <c r="D23" t="b">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
         <v>0.4</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F23" s="7">
         <v>2</v>
       </c>
-      <c r="G22" s="7">
-        <v>0</v>
-      </c>
-      <c r="H22" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="12">
+      <c r="G23" s="7">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="12">
         <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
-      <c r="J22" s="12">
+      <c r="J23" s="12">
         <f t="shared" si="6"/>
         <v>0.8</v>
       </c>
-      <c r="K22" s="2" t="s">
+      <c r="K23" s="2" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>341</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
         <v>342</v>
       </c>
-      <c r="D23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E23" s="1">
+      <c r="D24" t="b">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
         <v>0.86</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F24" s="7">
         <v>2</v>
       </c>
-      <c r="G23" s="7">
-        <v>0</v>
-      </c>
-      <c r="H23" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I23" s="12">
+      <c r="G24" s="7">
+        <v>0</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="12">
         <f t="shared" si="3"/>
         <v>1.72</v>
       </c>
-      <c r="J23" s="12">
+      <c r="J24" s="12">
         <f t="shared" si="6"/>
         <v>1.72</v>
       </c>
-      <c r="K23" s="2" t="s">
+      <c r="K24" s="2" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>358</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
         <v>359</v>
       </c>
-      <c r="D24" t="b">
-        <v>1</v>
-      </c>
-      <c r="E24" s="1">
+      <c r="D25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
         <v>1.02</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F25" s="7">
         <v>2</v>
       </c>
-      <c r="G24" s="7">
-        <v>0</v>
-      </c>
-      <c r="H24" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I24" s="12">
+      <c r="G25" s="7">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="12">
         <f t="shared" si="3"/>
         <v>2.04</v>
       </c>
-      <c r="J24" s="12">
+      <c r="J25" s="12">
         <f t="shared" si="6"/>
         <v>2.04</v>
       </c>
-      <c r="K24" s="2" t="s">
+      <c r="K25" s="2" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>344</v>
       </c>
-      <c r="B25">
+      <c r="B26">
         <v>16</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>347</v>
       </c>
-      <c r="D25" t="b">
-        <v>1</v>
-      </c>
-      <c r="E25" s="1">
+      <c r="D26" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1">
         <v>0.122</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F26" s="7">
         <v>100</v>
       </c>
-      <c r="G25" s="7">
-        <v>0</v>
-      </c>
-      <c r="H25" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I25" s="12">
+      <c r="G26" s="7">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="12">
         <f t="shared" si="3"/>
         <v>12.2</v>
       </c>
-      <c r="J25" s="12">
+      <c r="J26" s="12">
         <f t="shared" si="6"/>
         <v>12.2</v>
       </c>
-      <c r="K25" s="2" t="s">
+      <c r="K26" s="2" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>346</v>
       </c>
-      <c r="B26">
+      <c r="B27">
         <v>16</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>348</v>
       </c>
-      <c r="D26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E26" s="1">
+      <c r="D27" t="b">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1">
         <v>0.114</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F27" s="7">
         <v>100</v>
       </c>
-      <c r="G26" s="7">
-        <v>0</v>
-      </c>
-      <c r="H26" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I26" s="12">
+      <c r="G27" s="7">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="12">
         <f t="shared" si="3"/>
         <v>11.4</v>
       </c>
-      <c r="J26" s="12">
+      <c r="J27" s="12">
         <f t="shared" si="6"/>
         <v>11.4</v>
       </c>
-      <c r="K26" s="2" t="s">
+      <c r="K27" s="2" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>350</v>
       </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
         <v>351</v>
       </c>
-      <c r="D27" t="b">
-        <v>1</v>
-      </c>
-      <c r="E27" s="1">
+      <c r="D28" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1">
         <v>9.9499999999999993</v>
       </c>
-      <c r="F27" s="7">
-        <v>1</v>
-      </c>
-      <c r="G27" s="7">
-        <v>0</v>
-      </c>
-      <c r="H27" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I27" s="12">
+      <c r="F28" s="7">
+        <v>1</v>
+      </c>
+      <c r="G28" s="7">
+        <v>0</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="12">
         <f t="shared" si="3"/>
         <v>9.9499999999999993</v>
       </c>
-      <c r="J27" s="12">
+      <c r="J28" s="12">
         <f t="shared" si="6"/>
         <v>9.9499999999999993</v>
       </c>
-      <c r="K27" s="2" t="s">
+      <c r="K28" s="2" t="s">
         <v>349</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>353</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s">
-        <v>354</v>
-      </c>
-      <c r="D28" t="b">
-        <v>0</v>
-      </c>
-      <c r="E28" s="1">
-        <v>1</v>
-      </c>
-      <c r="F28" s="7">
-        <v>1</v>
-      </c>
-      <c r="G28" s="7">
-        <v>0</v>
-      </c>
-      <c r="H28" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I28" s="12">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J28" s="12">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D29" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29" s="1">
-        <v>8.9</v>
+        <v>1</v>
       </c>
       <c r="F29" s="7">
         <v>1</v>
@@ -3021,31 +3032,31 @@
       </c>
       <c r="I29" s="12">
         <f t="shared" si="3"/>
-        <v>8.9</v>
+        <v>0</v>
       </c>
       <c r="J29" s="12">
         <f t="shared" si="6"/>
-        <v>8.9</v>
+        <v>1</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D30" t="b">
         <v>1</v>
       </c>
       <c r="E30" s="1">
-        <v>89.54</v>
+        <v>8.9</v>
       </c>
       <c r="F30" s="7">
         <v>1</v>
@@ -3059,31 +3070,31 @@
       </c>
       <c r="I30" s="12">
         <f t="shared" si="3"/>
-        <v>89.54</v>
+        <v>8.9</v>
       </c>
       <c r="J30" s="12">
         <f t="shared" si="6"/>
-        <v>89.54</v>
+        <v>8.9</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>298</v>
+        <v>355</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="D31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" s="1">
-        <v>14.36</v>
+        <v>89.54</v>
       </c>
       <c r="F31" s="7">
         <v>1</v>
@@ -3097,49 +3108,87 @@
       </c>
       <c r="I31" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>89.54</v>
       </c>
       <c r="J31" s="12">
         <f t="shared" si="6"/>
+        <v>89.54</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>363</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>364</v>
+      </c>
+      <c r="D32" t="b">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
         <v>14.36</v>
       </c>
-      <c r="K31" s="2" t="s">
+      <c r="F32" s="7">
+        <v>1</v>
+      </c>
+      <c r="G32" s="7">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I32" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J32" s="12">
+        <f t="shared" si="6"/>
+        <v>14.36</v>
+      </c>
+      <c r="K32" s="2" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E32" s="1"/>
-      <c r="H32" s="1">
-        <f>SUM(H6:H31)</f>
-        <v>0</v>
-      </c>
-      <c r="I32" s="1">
-        <f>SUM(I6:I31)</f>
-        <v>2337.0700000000002</v>
-      </c>
-      <c r="J32" s="1">
-        <f>SUM(J6:J31)</f>
-        <v>2368.42</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+    <row r="33" spans="5:10" x14ac:dyDescent="0.2">
+      <c r="E33" s="1"/>
+      <c r="H33" s="1">
+        <f>SUM(H6:H32)</f>
+        <v>0</v>
+      </c>
+      <c r="I33" s="1">
+        <f>SUM(I6:I32)</f>
+        <v>2338.0700000000002</v>
+      </c>
+      <c r="J33" s="1">
+        <f>SUM(J6:J32)</f>
+        <v>2375.41</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>103</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K9" r:id="rId1" xr:uid="{B069B4F7-3B34-1F4D-91FE-BAFC3C3AFDEB}"/>
-    <hyperlink ref="K8" r:id="rId2" xr:uid="{A674AA42-7047-D742-B0B0-F79013D37D21}"/>
-    <hyperlink ref="K17" r:id="rId3" xr:uid="{933BC923-64A5-364D-B1D1-AA0CD0F86FE7}"/>
-    <hyperlink ref="K16" r:id="rId4" xr:uid="{040C449F-BD13-3A40-A3CF-B6CEB04C54CC}"/>
-    <hyperlink ref="K15" r:id="rId5" xr:uid="{1BE03111-1688-3547-8700-06A03759C772}"/>
-    <hyperlink ref="K22" r:id="rId6" xr:uid="{54E046B7-4373-0C4C-B1FF-977F5691AE73}"/>
+    <hyperlink ref="K10" r:id="rId1" xr:uid="{B069B4F7-3B34-1F4D-91FE-BAFC3C3AFDEB}"/>
+    <hyperlink ref="K9" r:id="rId2" xr:uid="{A674AA42-7047-D742-B0B0-F79013D37D21}"/>
+    <hyperlink ref="K18" r:id="rId3" xr:uid="{933BC923-64A5-364D-B1D1-AA0CD0F86FE7}"/>
+    <hyperlink ref="K17" r:id="rId4" xr:uid="{040C449F-BD13-3A40-A3CF-B6CEB04C54CC}"/>
+    <hyperlink ref="K16" r:id="rId5" xr:uid="{1BE03111-1688-3547-8700-06A03759C772}"/>
+    <hyperlink ref="K23" r:id="rId6" xr:uid="{54E046B7-4373-0C4C-B1FF-977F5691AE73}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updates BOM and adds more githubs.
</commit_message>
<xml_diff>
--- a/BOM/voron_2_tall_bom.xlsx
+++ b/BOM/voron_2_tall_bom.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ppak/GitHub/Voron-2-Tall/BOM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ppak1\GitHub\Voron-2-Tall\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986CA084-DA29-4F42-AC94-7EBADB5EBD72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1783CE05-B7B8-42AB-9B6B-733527D24DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="LDO_bom" sheetId="2" r:id="rId1"/>
-    <sheet name="white_orange_bom" sheetId="4" r:id="rId2"/>
-    <sheet name="self_source_bom" sheetId="1" r:id="rId3"/>
+    <sheet name="1_custom_kit" sheetId="2" r:id="rId1"/>
+    <sheet name="2_wiring" sheetId="5" r:id="rId2"/>
+    <sheet name="3_mods" sheetId="6" r:id="rId3"/>
+    <sheet name="theme_white_orange" sheetId="4" r:id="rId4"/>
+    <sheet name="reference_self_source" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="395">
   <si>
     <t>Category</t>
   </si>
@@ -949,12 +951,6 @@
     <t>LDO Kit already includes 5.9M</t>
   </si>
   <si>
-    <t>OVERATURE ABS Filament 1kg White</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/dp/B087M4P131?psc=1&amp;ref=ppx_yo2ov_dt_b_product_details</t>
-  </si>
-  <si>
     <t>Polymaker ABS Filament 1kg Orange</t>
   </si>
   <si>
@@ -970,9 +966,6 @@
     <t>Orange Acrylic Sheet 36" x 24" x 1/8" (3mm)</t>
   </si>
   <si>
-    <t>For General Printed Parts</t>
-  </si>
-  <si>
     <t>For Accented Printed Parts</t>
   </si>
   <si>
@@ -994,9 +987,6 @@
     <t>Door Panels (241.5x1103x3 mm)</t>
   </si>
   <si>
-    <t>LDO Kit + Custom Materials BOM</t>
-  </si>
-  <si>
     <t>Clear Acrylic Sheet 24" x 48" x 1/8"(4 Pack)</t>
   </si>
   <si>
@@ -1129,9 +1119,6 @@
     <t>NVME Base for Raspberry Pi 5</t>
   </si>
   <si>
-    <t>Optional Raspberry Pi storage expansion</t>
-  </si>
-  <si>
     <t>Required</t>
   </si>
   <si>
@@ -1159,10 +1146,82 @@
     <t>https://www.amazon.com/dp/B09B2CGW12?psc=1&amp;ref=ppx_yo2ov_dt_b_product_details</t>
   </si>
   <si>
-    <t>Pack of 100 (silver color to match theme)</t>
-  </si>
-  <si>
     <t>M3-0.5 x 8mm Socket Head Cap Screws Bolts</t>
+  </si>
+  <si>
+    <t>https://www.matterhackers.com/store/l/pro-series-abs/sk/MGY429XU</t>
+  </si>
+  <si>
+    <t>Natural PRO Series ABS Filament - 1.75mm (1kg)</t>
+  </si>
+  <si>
+    <t>For General Printed Parts (Whiteish Color)</t>
+  </si>
+  <si>
+    <t>Option 1: Extended LDO Wiring</t>
+  </si>
+  <si>
+    <t>Option 2: Canbus (Recommended)</t>
+  </si>
+  <si>
+    <t>Necessary Materials</t>
+  </si>
+  <si>
+    <t>Option 2: Canbus</t>
+  </si>
+  <si>
+    <t>1. LDO Kit + Custom Materials</t>
+  </si>
+  <si>
+    <t>3. Optional Modifications</t>
+  </si>
+  <si>
+    <t>2. Wiring</t>
+  </si>
+  <si>
+    <t>Frame Dimensions: 510mm x 510mm x 1130mm</t>
+  </si>
+  <si>
+    <t>Build Volume: 350mm x 350mm x (850mm to 930mm)</t>
+  </si>
+  <si>
+    <t>1. Raspberry Pi 5</t>
+  </si>
+  <si>
+    <t>Raspberry Pi 5 (8 Gb)</t>
+  </si>
+  <si>
+    <t>SC1112 Raspberry Pi | Mouser</t>
+  </si>
+  <si>
+    <t>Active Cooler</t>
+  </si>
+  <si>
+    <t>SC1148 Raspberry Pi | Mouser</t>
+  </si>
+  <si>
+    <t>Expected</t>
+  </si>
+  <si>
+    <t>Remaining</t>
+  </si>
+  <si>
+    <t>Subtotals</t>
+  </si>
+  <si>
+    <t>Upgrade from included Raspberry Pi 4</t>
+  </si>
+  <si>
+    <t>Necessary for Raspberry Pi 5</t>
+  </si>
+  <si>
+    <t>Allows for higher storage capacity</t>
+  </si>
+  <si>
+    <t>Note: Avoid using white ABS with Titanium Dioxide</t>
+  </si>
+  <si>
+    <t>Pack of 100</t>
   </si>
 </sst>
 </file>
@@ -1710,7 +1769,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
@@ -1724,6 +1783,8 @@
     <xf numFmtId="0" fontId="16" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="8" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1784,9 +1845,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1824,7 +1885,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1930,7 +1991,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2072,7 +2133,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2080,53 +2141,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F651F1D0-7A81-0546-9600-A8B0A78885C7}">
-  <dimension ref="A1:K84"/>
+  <dimension ref="A1:J68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="57.5" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
-    <col min="3" max="3" width="34.33203125" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.5" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" customWidth="1"/>
-    <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" customWidth="1"/>
-    <col min="9" max="9" width="9.83203125" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" customWidth="1"/>
-    <col min="11" max="11" width="18.1640625" customWidth="1"/>
+    <col min="3" max="3" width="34.375" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="7.375" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="10.375" customWidth="1"/>
+    <col min="8" max="8" width="9.875" customWidth="1"/>
+    <col min="9" max="9" width="10.375" customWidth="1"/>
+    <col min="10" max="10" width="18.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F4" s="8" t="s">
-        <v>368</v>
-      </c>
-      <c r="G4" s="9"/>
-      <c r="I4" s="10" t="s">
-        <v>366</v>
-      </c>
-      <c r="J4" s="11"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E4" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="H4" s="10" t="s">
+        <v>389</v>
+      </c>
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -2137,31 +2197,28 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>365</v>
       </c>
-      <c r="E5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>369</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>370</v>
-      </c>
-      <c r="H5" t="s">
-        <v>371</v>
+      <c r="G5" t="s">
+        <v>366</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>387</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>365</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>367</v>
-      </c>
-      <c r="K5" t="s">
+        <v>388</v>
+      </c>
+      <c r="J5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>299</v>
       </c>
@@ -2171,72 +2228,66 @@
       <c r="C6" t="s">
         <v>300</v>
       </c>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1">
+      <c r="D6" s="1">
         <v>1449</v>
       </c>
+      <c r="E6" s="7">
+        <v>1</v>
+      </c>
       <c r="F6" s="7">
-        <v>1</v>
-      </c>
-      <c r="G6" s="7">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1">
-        <f>G6*E6</f>
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <f>F6*D6</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="12">
+        <f xml:space="preserve"> D6*E6</f>
+        <v>1449</v>
       </c>
       <c r="I6" s="12">
-        <f t="shared" ref="I6:I10" si="0">IF(D6, E6*F6, E6*0)</f>
+        <f t="shared" ref="I6:I10" si="0">(E6-F6)*D6</f>
         <v>1449</v>
       </c>
-      <c r="J6" s="12">
-        <f t="shared" ref="J6:J10" si="1">(F6-G6)*E6</f>
-        <v>1449</v>
-      </c>
-      <c r="K6" t="s">
+      <c r="J6" s="2" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="B7">
         <v>100</v>
       </c>
       <c r="C7" t="s">
-        <v>374</v>
-      </c>
-      <c r="D7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
+        <v>394</v>
+      </c>
+      <c r="D7" s="1">
         <v>5.99</v>
       </c>
+      <c r="E7" s="7">
+        <v>1</v>
+      </c>
       <c r="F7" s="7">
-        <v>1</v>
-      </c>
-      <c r="G7" s="7">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="12">
+        <f t="shared" ref="H7:H15" si="1" xml:space="preserve"> D7*E7</f>
+        <v>5.99</v>
       </c>
       <c r="I7" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J7" s="12">
-        <f t="shared" si="1"/>
         <v>5.99</v>
       </c>
-      <c r="K7" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J7" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -2246,35 +2297,32 @@
       <c r="C8" t="s">
         <v>137</v>
       </c>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1">
+      <c r="D8" s="1">
         <v>12.88</v>
       </c>
+      <c r="E8" s="7">
+        <v>2</v>
+      </c>
       <c r="F8" s="7">
-        <v>2</v>
-      </c>
-      <c r="G8" s="7">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1">
-        <f t="shared" ref="H8:H32" si="2">G8*E8</f>
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" ref="G8:G16" si="2">F8*D8</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="12">
+        <f t="shared" si="1"/>
+        <v>25.76</v>
       </c>
       <c r="I8" s="12">
         <f t="shared" si="0"/>
         <v>25.76</v>
       </c>
-      <c r="J8" s="12">
-        <f t="shared" si="1"/>
-        <v>25.76</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="J8" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>302</v>
       </c>
@@ -2284,70 +2332,64 @@
       <c r="C9" t="s">
         <v>303</v>
       </c>
-      <c r="D9" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1">
+      <c r="D9" s="1">
         <v>30.91</v>
       </c>
+      <c r="E9" s="7">
+        <v>1</v>
+      </c>
       <c r="F9" s="7">
-        <v>1</v>
-      </c>
-      <c r="G9" s="7">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
+      </c>
+      <c r="H9" s="12">
+        <f t="shared" si="1"/>
+        <v>30.91</v>
       </c>
       <c r="I9" s="12">
         <f t="shared" si="0"/>
         <v>30.91</v>
       </c>
-      <c r="J9" s="12">
-        <f t="shared" si="1"/>
-        <v>30.91</v>
-      </c>
-      <c r="K9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>267</v>
       </c>
       <c r="B10">
         <v>4</v>
       </c>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" s="3">
+      <c r="D10" s="3">
         <v>66</v>
       </c>
+      <c r="E10" s="7">
+        <v>4</v>
+      </c>
       <c r="F10" s="7">
-        <v>4</v>
-      </c>
-      <c r="G10" s="7">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
+      </c>
+      <c r="H10" s="12">
+        <f t="shared" si="1"/>
+        <v>264</v>
       </c>
       <c r="I10" s="12">
         <f t="shared" si="0"/>
         <v>264</v>
       </c>
-      <c r="J10" s="12">
-        <f t="shared" si="1"/>
-        <v>264</v>
-      </c>
-      <c r="K10" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>274</v>
       </c>
@@ -2357,35 +2399,32 @@
       <c r="C11" t="s">
         <v>279</v>
       </c>
-      <c r="D11" t="b">
-        <v>1</v>
-      </c>
-      <c r="E11" s="1">
+      <c r="D11" s="1">
         <v>25.97</v>
       </c>
+      <c r="E11" s="7">
+        <v>4</v>
+      </c>
       <c r="F11" s="7">
-        <v>4</v>
-      </c>
-      <c r="G11" s="7">
-        <v>0</v>
-      </c>
-      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="H11" s="12">
+        <f t="shared" si="1"/>
+        <v>103.88</v>
+      </c>
       <c r="I11" s="12">
-        <f t="shared" ref="I11:I32" si="3">IF(D11, E11*F11, E11*0)</f>
+        <f t="shared" ref="I11" si="3">(E11-F11)*D11</f>
         <v>103.88</v>
       </c>
-      <c r="J11" s="12">
-        <f t="shared" ref="J11" si="4">(F11-G11)*E11</f>
-        <v>103.88</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="J11" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>78</v>
       </c>
@@ -2395,844 +2434,1245 @@
       <c r="C12" t="s">
         <v>281</v>
       </c>
-      <c r="D12" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" s="1">
+      <c r="D12" s="1">
         <v>8.99</v>
       </c>
+      <c r="E12" s="7">
+        <v>1</v>
+      </c>
       <c r="F12" s="7">
-        <v>1</v>
-      </c>
-      <c r="G12" s="7">
-        <v>0</v>
-      </c>
-      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="H12" s="12">
+        <f t="shared" si="1"/>
+        <v>8.99</v>
+      </c>
       <c r="I12" s="12">
-        <f t="shared" si="3"/>
+        <f>(E12-F12)*D12</f>
         <v>8.99</v>
       </c>
-      <c r="J12" s="12">
-        <f>(F12-G12)*E12</f>
-        <v>8.99</v>
-      </c>
-      <c r="K12" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J12" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>296</v>
+        <v>276</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>297</v>
-      </c>
-      <c r="D13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1">
-        <v>89.54</v>
+        <v>277</v>
+      </c>
+      <c r="D13" s="1">
+        <v>46.44</v>
+      </c>
+      <c r="E13" s="7">
+        <v>1</v>
       </c>
       <c r="F13" s="7">
-        <v>1</v>
-      </c>
-      <c r="G13" s="7">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="H13" s="12">
+        <f t="shared" si="1"/>
+        <v>46.44</v>
+      </c>
       <c r="I13" s="12">
-        <f t="shared" si="3"/>
-        <v>89.54</v>
-      </c>
-      <c r="J13" s="12">
-        <f t="shared" ref="J13:J15" si="5">(F13-G13)*E13</f>
-        <v>89.54</v>
-      </c>
-      <c r="K13" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+        <f t="shared" ref="I13:I15" si="4">(E13-F13)*D13</f>
+        <v>46.44</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B14">
-        <v>28</v>
-      </c>
-      <c r="C14" t="s">
-        <v>294</v>
-      </c>
-      <c r="D14" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1">
-        <v>8.3000000000000004E-2</v>
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>6.12</v>
+      </c>
+      <c r="E14" s="7">
+        <v>1</v>
       </c>
       <c r="F14" s="7">
-        <v>100</v>
-      </c>
-      <c r="G14" s="7">
-        <v>0</v>
-      </c>
-      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="H14" s="12">
+        <f t="shared" si="1"/>
+        <v>6.12</v>
+      </c>
       <c r="I14" s="12">
-        <f t="shared" si="3"/>
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="J14" s="12">
-        <f t="shared" si="5"/>
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="K14" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>6.12</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>292</v>
+        <v>316</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>293</v>
-      </c>
-      <c r="D15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1">
-        <v>1.02</v>
+        <v>314</v>
+      </c>
+      <c r="D15" s="1">
+        <v>139.80000000000001</v>
+      </c>
+      <c r="E15" s="7">
+        <v>1</v>
       </c>
       <c r="F15" s="7">
-        <v>2</v>
-      </c>
-      <c r="G15" s="7">
-        <v>0</v>
-      </c>
-      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="H15" s="12">
+        <f t="shared" si="1"/>
+        <v>139.80000000000001</v>
+      </c>
       <c r="I15" s="12">
-        <f t="shared" si="3"/>
-        <v>2.04</v>
-      </c>
-      <c r="J15" s="12">
-        <f t="shared" si="5"/>
-        <v>2.04</v>
-      </c>
-      <c r="K15" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>276</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
+        <f t="shared" si="4"/>
+        <v>139.80000000000001</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>277</v>
-      </c>
-      <c r="D16" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" s="1">
-        <v>46.44</v>
-      </c>
-      <c r="F16" s="7">
-        <v>1</v>
-      </c>
-      <c r="G16" s="7">
-        <v>0</v>
-      </c>
-      <c r="H16" s="1">
+        <v>315</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I16" s="12">
-        <f t="shared" si="3"/>
-        <v>46.44</v>
-      </c>
-      <c r="J16" s="12">
-        <f t="shared" ref="J16:J32" si="6">(F16-G16)*E16</f>
-        <v>46.44</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>101</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="D17" t="b">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1">
-        <v>6.12</v>
-      </c>
-      <c r="F17" s="7">
-        <v>1</v>
-      </c>
-      <c r="G17" s="7">
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="1"/>
+      <c r="G17" s="1">
+        <f>SUM(G6:G16)</f>
         <v>0</v>
       </c>
       <c r="H17" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="12">
-        <f t="shared" si="3"/>
-        <v>6.12</v>
-      </c>
-      <c r="J17" s="12">
-        <f t="shared" si="6"/>
-        <v>6.12</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>320</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>317</v>
-      </c>
-      <c r="D18" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" s="1">
-        <v>139.80000000000001</v>
-      </c>
-      <c r="F18" s="7">
-        <v>1</v>
-      </c>
-      <c r="G18" s="7">
-        <v>0</v>
-      </c>
-      <c r="H18" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="12">
-        <f t="shared" si="3"/>
-        <v>139.80000000000001</v>
-      </c>
-      <c r="J18" s="12">
-        <f t="shared" si="6"/>
-        <v>139.80000000000001</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
-        <v>318</v>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>330</v>
-      </c>
-      <c r="B20">
-        <v>2</v>
-      </c>
-      <c r="C20" t="s">
-        <v>332</v>
-      </c>
-      <c r="D20" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20" s="1">
-        <v>12.99</v>
-      </c>
-      <c r="F20" s="7">
-        <v>2</v>
-      </c>
-      <c r="G20" s="7">
-        <v>0</v>
-      </c>
-      <c r="H20" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I20" s="12">
-        <f t="shared" si="3"/>
-        <v>25.98</v>
-      </c>
-      <c r="J20" s="12">
-        <f t="shared" si="6"/>
-        <v>25.98</v>
-      </c>
-      <c r="K20" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>328</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21" t="s">
-        <v>329</v>
-      </c>
-      <c r="D21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E21" s="1">
-        <v>15.99</v>
-      </c>
-      <c r="F21" s="7">
-        <v>1</v>
-      </c>
-      <c r="G21" s="7">
-        <v>0</v>
-      </c>
-      <c r="H21" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I21" s="12">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J21" s="12">
-        <f t="shared" si="6"/>
-        <v>15.99</v>
-      </c>
-      <c r="K21" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>338</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
-        <v>336</v>
-      </c>
-      <c r="D22" t="b">
-        <v>1</v>
-      </c>
-      <c r="E22" s="1">
-        <v>0.38</v>
-      </c>
-      <c r="F22" s="7">
-        <v>2</v>
-      </c>
-      <c r="G22" s="7">
-        <v>0</v>
-      </c>
-      <c r="H22" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="12">
-        <f t="shared" si="3"/>
-        <v>0.76</v>
-      </c>
-      <c r="J22" s="12">
-        <f t="shared" si="6"/>
-        <v>0.76</v>
-      </c>
-      <c r="K22" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>339</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
-        <v>337</v>
-      </c>
-      <c r="D23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E23" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="F23" s="7">
-        <v>2</v>
-      </c>
-      <c r="G23" s="7">
-        <v>0</v>
-      </c>
-      <c r="H23" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I23" s="12">
-        <f t="shared" si="3"/>
-        <v>0.8</v>
-      </c>
-      <c r="J23" s="12">
-        <f t="shared" si="6"/>
-        <v>0.8</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>341</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
-        <v>342</v>
-      </c>
-      <c r="D24" t="b">
-        <v>1</v>
-      </c>
-      <c r="E24" s="1">
-        <v>0.86</v>
-      </c>
-      <c r="F24" s="7">
-        <v>2</v>
-      </c>
-      <c r="G24" s="7">
-        <v>0</v>
-      </c>
-      <c r="H24" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I24" s="12">
-        <f t="shared" si="3"/>
-        <v>1.72</v>
-      </c>
-      <c r="J24" s="12">
-        <f t="shared" si="6"/>
-        <v>1.72</v>
-      </c>
-      <c r="K24" s="2" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>358</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
-        <v>359</v>
-      </c>
-      <c r="D25" t="b">
-        <v>1</v>
-      </c>
-      <c r="E25" s="1">
-        <v>1.02</v>
-      </c>
-      <c r="F25" s="7">
-        <v>2</v>
-      </c>
-      <c r="G25" s="7">
-        <v>0</v>
-      </c>
-      <c r="H25" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I25" s="12">
-        <f t="shared" si="3"/>
-        <v>2.04</v>
-      </c>
-      <c r="J25" s="12">
-        <f t="shared" si="6"/>
-        <v>2.04</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>344</v>
-      </c>
-      <c r="B26">
-        <v>16</v>
-      </c>
-      <c r="C26" t="s">
-        <v>347</v>
-      </c>
-      <c r="D26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E26" s="1">
-        <v>0.122</v>
-      </c>
-      <c r="F26" s="7">
-        <v>100</v>
-      </c>
-      <c r="G26" s="7">
-        <v>0</v>
-      </c>
-      <c r="H26" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I26" s="12">
-        <f t="shared" si="3"/>
-        <v>12.2</v>
-      </c>
-      <c r="J26" s="12">
-        <f t="shared" si="6"/>
-        <v>12.2</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>346</v>
-      </c>
-      <c r="B27">
-        <v>16</v>
-      </c>
-      <c r="C27" t="s">
-        <v>348</v>
-      </c>
-      <c r="D27" t="b">
-        <v>1</v>
-      </c>
-      <c r="E27" s="1">
-        <v>0.114</v>
-      </c>
-      <c r="F27" s="7">
-        <v>100</v>
-      </c>
-      <c r="G27" s="7">
-        <v>0</v>
-      </c>
-      <c r="H27" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I27" s="12">
-        <f t="shared" si="3"/>
-        <v>11.4</v>
-      </c>
-      <c r="J27" s="12">
-        <f t="shared" si="6"/>
-        <v>11.4</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>350</v>
-      </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s">
-        <v>351</v>
-      </c>
-      <c r="D28" t="b">
-        <v>1</v>
-      </c>
-      <c r="E28" s="1">
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="F28" s="7">
-        <v>1</v>
-      </c>
-      <c r="G28" s="7">
-        <v>0</v>
-      </c>
-      <c r="H28" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I28" s="12">
-        <f t="shared" si="3"/>
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="J28" s="12">
-        <f t="shared" si="6"/>
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>353</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29" t="s">
-        <v>354</v>
-      </c>
-      <c r="D29" t="b">
-        <v>0</v>
-      </c>
-      <c r="E29" s="1">
-        <v>1</v>
-      </c>
-      <c r="F29" s="7">
-        <v>1</v>
-      </c>
-      <c r="G29" s="7">
-        <v>0</v>
-      </c>
-      <c r="H29" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I29" s="12">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J29" s="12">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>356</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
-        <v>357</v>
-      </c>
-      <c r="D30" t="b">
-        <v>1</v>
-      </c>
-      <c r="E30" s="1">
-        <v>8.9</v>
-      </c>
-      <c r="F30" s="7">
-        <v>1</v>
-      </c>
-      <c r="G30" s="7">
-        <v>0</v>
-      </c>
-      <c r="H30" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I30" s="12">
-        <f t="shared" si="3"/>
-        <v>8.9</v>
-      </c>
-      <c r="J30" s="12">
-        <f t="shared" si="6"/>
-        <v>8.9</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>360</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
-        <v>361</v>
-      </c>
-      <c r="D31" t="b">
-        <v>1</v>
-      </c>
-      <c r="E31" s="1">
-        <v>89.54</v>
-      </c>
-      <c r="F31" s="7">
-        <v>1</v>
-      </c>
-      <c r="G31" s="7">
-        <v>0</v>
-      </c>
-      <c r="H31" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I31" s="12">
-        <f t="shared" si="3"/>
-        <v>89.54</v>
-      </c>
-      <c r="J31" s="12">
-        <f t="shared" si="6"/>
-        <v>89.54</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>363</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s">
-        <v>364</v>
-      </c>
-      <c r="D32" t="b">
-        <v>0</v>
-      </c>
-      <c r="E32" s="1">
-        <v>14.36</v>
-      </c>
-      <c r="F32" s="7">
-        <v>1</v>
-      </c>
-      <c r="G32" s="7">
-        <v>0</v>
-      </c>
-      <c r="H32" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I32" s="12">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J32" s="12">
-        <f t="shared" si="6"/>
-        <v>14.36</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="33" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E33" s="1"/>
-      <c r="H33" s="1">
-        <f>SUM(H6:H32)</f>
-        <v>0</v>
-      </c>
-      <c r="I33" s="1">
-        <f>SUM(I6:I32)</f>
-        <v>2338.0700000000002</v>
-      </c>
-      <c r="J33" s="1">
-        <f>SUM(J6:J32)</f>
-        <v>2375.41</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+        <f>SUM(H6:H16)</f>
+        <v>2080.89</v>
+      </c>
+      <c r="I17" s="1">
+        <f>SUM(I6:I16)</f>
+        <v>2080.89</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>103</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K10" r:id="rId1" xr:uid="{B069B4F7-3B34-1F4D-91FE-BAFC3C3AFDEB}"/>
-    <hyperlink ref="K9" r:id="rId2" xr:uid="{A674AA42-7047-D742-B0B0-F79013D37D21}"/>
-    <hyperlink ref="K18" r:id="rId3" xr:uid="{933BC923-64A5-364D-B1D1-AA0CD0F86FE7}"/>
-    <hyperlink ref="K17" r:id="rId4" xr:uid="{040C449F-BD13-3A40-A3CF-B6CEB04C54CC}"/>
-    <hyperlink ref="K16" r:id="rId5" xr:uid="{1BE03111-1688-3547-8700-06A03759C772}"/>
-    <hyperlink ref="K23" r:id="rId6" xr:uid="{54E046B7-4373-0C4C-B1FF-977F5691AE73}"/>
+    <hyperlink ref="J10" r:id="rId1" xr:uid="{B069B4F7-3B34-1F4D-91FE-BAFC3C3AFDEB}"/>
+    <hyperlink ref="J9" r:id="rId2" xr:uid="{A674AA42-7047-D742-B0B0-F79013D37D21}"/>
+    <hyperlink ref="J15" r:id="rId3" xr:uid="{933BC923-64A5-364D-B1D1-AA0CD0F86FE7}"/>
+    <hyperlink ref="J14" r:id="rId4" xr:uid="{040C449F-BD13-3A40-A3CF-B6CEB04C54CC}"/>
+    <hyperlink ref="J13" r:id="rId5" xr:uid="{1BE03111-1688-3547-8700-06A03759C772}"/>
+    <hyperlink ref="J6" r:id="rId6" xr:uid="{95771CD4-335F-4BC9-AC44-BA0B6FF377F1}"/>
+    <hyperlink ref="J12" r:id="rId7" xr:uid="{9C5256D3-4225-4D6A-9A4B-B2579A49D423}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4686087C-B58C-7A42-AAAC-3D022FB0521D}">
-  <dimension ref="A1:K67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B333F01F-4973-487B-89AC-950BB7EE7FAF}">
+  <dimension ref="A1:J60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="82.5" customWidth="1"/>
+    <col min="1" max="1" width="57.5" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
-    <col min="3" max="3" width="36.33203125" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.5" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" customWidth="1"/>
-    <col min="9" max="9" width="12.5" customWidth="1"/>
-    <col min="10" max="10" width="16.1640625" customWidth="1"/>
-    <col min="11" max="11" width="18.1640625" customWidth="1"/>
+    <col min="3" max="3" width="34.375" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="7.375" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="10.375" customWidth="1"/>
+    <col min="8" max="8" width="9.875" customWidth="1"/>
+    <col min="9" max="9" width="10.375" customWidth="1"/>
+    <col min="10" max="10" width="18.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>375</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="H6" s="10" t="s">
+        <v>389</v>
+      </c>
+      <c r="I6" s="11"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>254</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="G7" t="s">
+        <v>366</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>387</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>388</v>
+      </c>
+      <c r="J7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>326</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>328</v>
+      </c>
+      <c r="D8" s="1">
+        <v>12.99</v>
+      </c>
+      <c r="E8" s="7">
+        <v>2</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" ref="G8:G9" si="0">F8*D8</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="12">
+        <f>D8*E8</f>
+        <v>25.98</v>
+      </c>
+      <c r="I8" s="12">
+        <f t="shared" ref="I8:I9" si="1">(E8-F8)*D8</f>
+        <v>25.98</v>
+      </c>
+      <c r="J8" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>346</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>347</v>
+      </c>
+      <c r="D9" s="1">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="12">
+        <f>D9*E9</f>
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="I9" s="12">
+        <f t="shared" si="1"/>
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D10" s="1"/>
+      <c r="G10" s="1">
+        <f>SUM(G8:G9)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <f>SUM(H8:H9)</f>
+        <v>35.93</v>
+      </c>
+      <c r="I10" s="1">
+        <f>SUM(I8:I9)</f>
+        <v>35.93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>373</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="H12" s="10" t="s">
+        <v>361</v>
+      </c>
+      <c r="I12" s="11"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>254</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="G13" t="s">
+        <v>366</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>362</v>
+      </c>
+      <c r="J13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>294</v>
+      </c>
+      <c r="D14" s="1">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="E14" s="7">
+        <v>100</v>
+      </c>
+      <c r="F14" s="7">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <f>F14*D14</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="12">
+        <f>D14*E14</f>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="I14" s="12">
+        <f>(E14-F14)*D14</f>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="J14" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>292</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>293</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1.02</v>
+      </c>
+      <c r="E15" s="7">
+        <v>2</v>
+      </c>
+      <c r="F15" s="7">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <f>F15*D15</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="12">
+        <f t="shared" ref="H15:H23" si="2">D15*E15</f>
+        <v>2.04</v>
+      </c>
+      <c r="I15" s="12">
+        <f>(E15-F15)*D15</f>
+        <v>2.04</v>
+      </c>
+      <c r="J15" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>334</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>332</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="E16" s="7">
+        <v>2</v>
+      </c>
+      <c r="F16" s="7">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <f>F16*D16</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="12">
+        <f t="shared" si="2"/>
+        <v>0.76</v>
+      </c>
+      <c r="I16" s="12">
+        <f>(E16-F16)*D16</f>
+        <v>0.76</v>
+      </c>
+      <c r="J16" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>335</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>333</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="E17" s="7">
+        <v>2</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <f>F17*D17</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="12">
+        <f t="shared" si="2"/>
+        <v>0.8</v>
+      </c>
+      <c r="I17" s="12">
+        <f>(E17-F17)*D17</f>
+        <v>0.8</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>337</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>338</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="E18" s="7">
+        <v>2</v>
+      </c>
+      <c r="F18" s="7">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <f>F18*D18</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="12">
+        <f t="shared" si="2"/>
+        <v>1.72</v>
+      </c>
+      <c r="I18" s="12">
+        <f>(E18-F18)*D18</f>
+        <v>1.72</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>354</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>355</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1.02</v>
+      </c>
+      <c r="E19" s="7">
+        <v>2</v>
+      </c>
+      <c r="F19" s="7">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <f>F19*D19</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="12">
+        <f t="shared" si="2"/>
+        <v>2.04</v>
+      </c>
+      <c r="I19" s="12">
+        <f>(E19-F19)*D19</f>
+        <v>2.04</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>340</v>
+      </c>
+      <c r="B20">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>343</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.122</v>
+      </c>
+      <c r="E20" s="7">
+        <v>100</v>
+      </c>
+      <c r="F20" s="7">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <f>F20*D20</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="12">
+        <f t="shared" si="2"/>
+        <v>12.2</v>
+      </c>
+      <c r="I20" s="12">
+        <f>(E20-F20)*D20</f>
+        <v>12.2</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>342</v>
+      </c>
+      <c r="B21">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
+        <v>344</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.114</v>
+      </c>
+      <c r="E21" s="7">
+        <v>100</v>
+      </c>
+      <c r="F21" s="7">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <f>F21*D21</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="12">
+        <f t="shared" si="2"/>
+        <v>11.4</v>
+      </c>
+      <c r="I21" s="12">
+        <f>(E21-F21)*D21</f>
+        <v>11.4</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>356</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>357</v>
+      </c>
+      <c r="D22" s="1">
+        <v>89.54</v>
+      </c>
+      <c r="E22" s="7">
+        <v>1</v>
+      </c>
+      <c r="F22" s="7">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
+        <f>F22*D22</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="12">
+        <f t="shared" si="2"/>
+        <v>89.54</v>
+      </c>
+      <c r="I22" s="12">
+        <f>(E22-F22)*D22</f>
+        <v>89.54</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>352</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>353</v>
+      </c>
+      <c r="D23" s="1">
+        <v>8.9</v>
+      </c>
+      <c r="E23" s="7">
+        <v>1</v>
+      </c>
+      <c r="F23" s="7">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1">
+        <f>F23*D23</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="12">
+        <f t="shared" si="2"/>
+        <v>8.9</v>
+      </c>
+      <c r="I23" s="12">
+        <f>(E23-F23)*D23</f>
+        <v>8.9</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G24" s="1">
+        <f>SUM(G14:G23)</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="1">
+        <f>SUM(H14:H23)</f>
+        <v>137.70000000000002</v>
+      </c>
+      <c r="I24" s="1">
+        <f>SUM(I14:I23)</f>
+        <v>137.70000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>376</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="F26" s="9"/>
+      <c r="H26" s="10" t="s">
+        <v>361</v>
+      </c>
+      <c r="I26" s="11"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>254</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>114</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="G27" t="s">
+        <v>366</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>362</v>
+      </c>
+      <c r="J27" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28">
+        <v>28</v>
+      </c>
+      <c r="C28" t="s">
+        <v>294</v>
+      </c>
+      <c r="D28" s="1">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="E28" s="7">
+        <v>100</v>
+      </c>
+      <c r="F28" s="7">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1">
+        <f>F28*D28</f>
+        <v>0</v>
+      </c>
+      <c r="H28" s="12">
+        <f>D28*E28</f>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="I28" s="12">
+        <f>(E28-F28)*D28</f>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="J28" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>292</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>293</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1.02</v>
+      </c>
+      <c r="E29" s="7">
+        <v>2</v>
+      </c>
+      <c r="F29" s="7">
+        <v>0</v>
+      </c>
+      <c r="G29" s="1">
+        <f>F29*D29</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="12">
+        <f t="shared" ref="H29:H37" si="3">D29*E29</f>
+        <v>2.04</v>
+      </c>
+      <c r="I29" s="12">
+        <f>(E29-F29)*D29</f>
+        <v>2.04</v>
+      </c>
+      <c r="J29" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>334</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>332</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="E30" s="7">
+        <v>2</v>
+      </c>
+      <c r="F30" s="7">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1">
+        <f>F30*D30</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="12">
+        <f t="shared" si="3"/>
+        <v>0.76</v>
+      </c>
+      <c r="I30" s="12">
+        <f>(E30-F30)*D30</f>
+        <v>0.76</v>
+      </c>
+      <c r="J30" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>335</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>333</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="E31" s="7">
+        <v>2</v>
+      </c>
+      <c r="F31" s="7">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1">
+        <f>F31*D31</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="12">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
+      <c r="I31" s="12">
+        <f>(E31-F31)*D31</f>
+        <v>0.8</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>337</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>338</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="E32" s="7">
+        <v>2</v>
+      </c>
+      <c r="F32" s="7">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1">
+        <f>F32*D32</f>
+        <v>0</v>
+      </c>
+      <c r="H32" s="12">
+        <f t="shared" si="3"/>
+        <v>1.72</v>
+      </c>
+      <c r="I32" s="12">
+        <f>(E32-F32)*D32</f>
+        <v>1.72</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>354</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>355</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1.02</v>
+      </c>
+      <c r="E33" s="7">
+        <v>2</v>
+      </c>
+      <c r="F33" s="7">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1">
+        <f>F33*D33</f>
+        <v>0</v>
+      </c>
+      <c r="H33" s="12">
+        <f t="shared" si="3"/>
+        <v>2.04</v>
+      </c>
+      <c r="I33" s="12">
+        <f>(E33-F33)*D33</f>
+        <v>2.04</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>340</v>
+      </c>
+      <c r="B34">
+        <v>16</v>
+      </c>
+      <c r="C34" t="s">
+        <v>343</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0.122</v>
+      </c>
+      <c r="E34" s="7">
+        <v>100</v>
+      </c>
+      <c r="F34" s="7">
+        <v>0</v>
+      </c>
+      <c r="G34" s="1">
+        <f>F34*D34</f>
+        <v>0</v>
+      </c>
+      <c r="H34" s="12">
+        <f t="shared" si="3"/>
+        <v>12.2</v>
+      </c>
+      <c r="I34" s="12">
+        <f>(E34-F34)*D34</f>
+        <v>12.2</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>342</v>
+      </c>
+      <c r="B35">
+        <v>16</v>
+      </c>
+      <c r="C35" t="s">
+        <v>344</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0.114</v>
+      </c>
+      <c r="E35" s="7">
+        <v>100</v>
+      </c>
+      <c r="F35" s="7">
+        <v>0</v>
+      </c>
+      <c r="G35" s="1">
+        <f>F35*D35</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="12">
+        <f t="shared" si="3"/>
+        <v>11.4</v>
+      </c>
+      <c r="I35" s="12">
+        <f>(E35-F35)*D35</f>
+        <v>11.4</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>356</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>357</v>
+      </c>
+      <c r="D36" s="1">
+        <v>89.54</v>
+      </c>
+      <c r="E36" s="7">
+        <v>1</v>
+      </c>
+      <c r="F36" s="7">
+        <v>0</v>
+      </c>
+      <c r="G36" s="1">
+        <f>F36*D36</f>
+        <v>0</v>
+      </c>
+      <c r="H36" s="12">
+        <f t="shared" si="3"/>
+        <v>89.54</v>
+      </c>
+      <c r="I36" s="12">
+        <f>(E36-F36)*D36</f>
+        <v>89.54</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>352</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>353</v>
+      </c>
+      <c r="D37" s="1">
+        <v>8.9</v>
+      </c>
+      <c r="E37" s="7">
+        <v>1</v>
+      </c>
+      <c r="F37" s="7">
+        <v>0</v>
+      </c>
+      <c r="G37" s="1">
+        <f>F37*D37</f>
+        <v>0</v>
+      </c>
+      <c r="H37" s="12">
+        <f t="shared" si="3"/>
+        <v>8.9</v>
+      </c>
+      <c r="I37" s="12">
+        <f>(E37-F37)*D37</f>
+        <v>8.9</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G38" s="1">
+        <f>SUM(G28:G37)</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="1">
+        <f>SUM(H28:H37)</f>
+        <v>137.70000000000002</v>
+      </c>
+      <c r="I38" s="1">
+        <f>SUM(I28:I37)</f>
+        <v>137.70000000000002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J17" r:id="rId1" xr:uid="{8F88ED9B-1C89-4651-AF81-0D0D1136F20A}"/>
+    <hyperlink ref="J31" r:id="rId2" xr:uid="{6D16E149-47DE-4D84-AA2C-CEB7B48F918E}"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{645409AD-79BA-4214-8D29-3BF242B131B1}">
+  <dimension ref="A1:J63"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="57.5" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="34.375" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="7.375" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="10.375" customWidth="1"/>
+    <col min="8" max="8" width="9.875" customWidth="1"/>
+    <col min="9" max="9" width="10.375" customWidth="1"/>
+    <col min="10" max="10" width="18.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>382</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="H4" s="10" t="s">
+        <v>389</v>
+      </c>
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -3243,383 +3683,550 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>200</v>
-      </c>
-      <c r="E5" t="s">
         <v>114</v>
       </c>
-      <c r="F5" t="s">
-        <v>252</v>
+      <c r="E5" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>365</v>
       </c>
       <c r="G5" t="s">
-        <v>253</v>
-      </c>
-      <c r="H5" t="s">
-        <v>199</v>
-      </c>
-      <c r="I5" t="s">
-        <v>198</v>
+        <v>366</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>387</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>388</v>
       </c>
       <c r="J5" t="s">
-        <v>223</v>
-      </c>
-      <c r="K5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>283</v>
+        <v>383</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>285</v>
-      </c>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1">
-        <v>7.24</v>
-      </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1">
-        <f t="shared" ref="H6:H7" si="0">IF(NOT(D6), E6*F6, E6*0)</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="1">
-        <f t="shared" ref="I6:I14" si="1">IF(D6, E6*F6, E6*0)</f>
-        <v>14.48</v>
-      </c>
-      <c r="J6" s="1">
-        <f t="shared" ref="J6:J15" si="2">(F6-G6)*E6</f>
-        <v>14.48</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+        <v>390</v>
+      </c>
+      <c r="D6" s="1">
+        <v>80</v>
+      </c>
+      <c r="E6" s="7">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <f>F6*D6</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="12">
+        <f>D6*E6</f>
+        <v>80</v>
+      </c>
+      <c r="I6" s="12">
+        <f>(E6-F6)*D6</f>
+        <v>80</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>286</v>
+        <v>385</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>287</v>
-      </c>
-      <c r="D7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1">
-        <v>7.7</v>
-      </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1">
+        <v>391</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <f>F7*D7</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="12">
+        <f>D7*E7</f>
+        <v>5</v>
+      </c>
+      <c r="I7" s="12">
+        <f>(E7-F7)*D7</f>
+        <v>5</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>324</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>325</v>
+      </c>
+      <c r="D8" s="1">
+        <v>15.99</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <f>F8*D8</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="12">
+        <f t="shared" ref="H8:H10" si="0">D8*E8</f>
+        <v>15.99</v>
+      </c>
+      <c r="I8" s="12">
+        <f>(E8-F8)*D8</f>
+        <v>15.99</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>349</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>350</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <f>F9*D9</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I7" s="1">
-        <f t="shared" si="1"/>
-        <v>15.4</v>
-      </c>
-      <c r="J7" s="1">
-        <f t="shared" si="2"/>
-        <v>15.4</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>310</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>316</v>
-      </c>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1">
-        <v>24.95</v>
-      </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1">
-        <f t="shared" si="1"/>
-        <v>49.9</v>
-      </c>
-      <c r="J8" s="1">
-        <f t="shared" si="2"/>
-        <v>49.9</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
-        <v>315</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I9" s="12">
+        <f>(E9-F9)*D9</f>
+        <v>1</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>324</v>
+        <v>359</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>308</v>
-      </c>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1">
-        <v>49.95</v>
-      </c>
-      <c r="F10">
-        <v>4</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1">
-        <f t="shared" ref="H10:H14" si="3">IF(NOT(D10), E10*F10, E10*0)</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="1">
-        <f t="shared" si="1"/>
-        <v>199.8</v>
-      </c>
-      <c r="J10" s="1">
-        <f t="shared" si="2"/>
-        <v>199.8</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C11" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>304</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>311</v>
-      </c>
-      <c r="D12" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" s="1">
-        <v>19.989999999999998</v>
-      </c>
-      <c r="F12">
-        <v>2</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="1">
-        <f t="shared" si="1"/>
-        <v>39.979999999999997</v>
-      </c>
-      <c r="J12" s="1">
-        <f t="shared" si="2"/>
-        <v>39.979999999999997</v>
-      </c>
-      <c r="K12" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>306</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>312</v>
-      </c>
-      <c r="D13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1">
-        <v>21.99</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="1">
-        <f t="shared" si="1"/>
-        <v>21.99</v>
-      </c>
-      <c r="J13" s="1">
-        <f t="shared" si="2"/>
-        <v>21.99</v>
-      </c>
-      <c r="K13" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>333</v>
-      </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>325</v>
-      </c>
-      <c r="D14" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1">
-        <v>12.94</v>
-      </c>
-      <c r="F14">
-        <v>2</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I14" s="1">
-        <f t="shared" si="1"/>
-        <v>25.88</v>
-      </c>
-      <c r="J14" s="1">
-        <f t="shared" si="2"/>
-        <v>25.88</v>
-      </c>
-      <c r="K14" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>290</v>
-      </c>
-      <c r="B15">
-        <v>8</v>
-      </c>
-      <c r="C15" t="s">
-        <v>313</v>
-      </c>
-      <c r="D15" t="b">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1">
-        <v>6.04</v>
-      </c>
-      <c r="F15">
-        <v>8</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15" s="1">
-        <f t="shared" ref="H15" si="4">IF(NOT(D15), E15*F15, E15*0)</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="1">
-        <f t="shared" ref="I15" si="5">IF(D15, E15*F15, E15*0)</f>
-        <v>48.32</v>
-      </c>
-      <c r="J15" s="1">
-        <f t="shared" si="2"/>
-        <v>48.32</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H16" s="1">
+        <v>392</v>
+      </c>
+      <c r="D10" s="1">
+        <v>14.36</v>
+      </c>
+      <c r="E10" s="7">
+        <v>1</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <f>F10*D10</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="12">
+        <f t="shared" si="0"/>
+        <v>14.36</v>
+      </c>
+      <c r="I10" s="12">
+        <f>(E10-F10)*D10</f>
+        <v>14.36</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
+      <c r="G11" s="1">
+        <f>SUM(G8:G10)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="14">
         <f>SUM(H6:H10)</f>
-        <v>0</v>
-      </c>
-      <c r="I16" s="1">
-        <f>SUM(I6:I15)</f>
-        <v>415.75000000000006</v>
-      </c>
-      <c r="J16" s="1">
-        <f>SUM(J6:J15)</f>
-        <v>415.75000000000006</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+        <v>116.35</v>
+      </c>
+      <c r="I11" s="1">
+        <f>SUM(I6:I10)</f>
+        <v>116.35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>103</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K10" r:id="rId1" xr:uid="{D015C5EB-6B16-0744-8964-924D048D7799}"/>
-    <hyperlink ref="K8" r:id="rId2" xr:uid="{87546791-3990-2846-B60F-64D77FF64AB4}"/>
-    <hyperlink ref="K15" r:id="rId3" xr:uid="{8FEB2D40-243D-EB40-9049-84074FF0142B}"/>
+    <hyperlink ref="J6" r:id="rId1" display="https://www.mouser.com/ProductDetail/Raspberry-Pi/SC1112?qs=HoCaDK9Nz5c86n0i5EQ%2FPA%3D%3D" xr:uid="{1AD7AD03-BA63-4D8F-89EC-00A7DFC89138}"/>
+    <hyperlink ref="J7" r:id="rId2" display="https://www.mouser.com/ProductDetail/Raspberry-Pi/SC1148?qs=HoCaDK9Nz5fqo0izK2taew%3D%3D" xr:uid="{3B3FFB0D-A2AF-4610-B56A-77263F3DF5B7}"/>
+    <hyperlink ref="J8" r:id="rId3" xr:uid="{64585390-A70C-4A01-8458-C19F01A4A832}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4686087C-B58C-7A42-AAAC-3D022FB0521D}">
+  <dimension ref="A1:H66"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="82.5" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="36.375" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="16.125" customWidth="1"/>
+    <col min="8" max="8" width="18.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="6" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" t="s">
+        <v>252</v>
+      </c>
+      <c r="F4" t="s">
+        <v>253</v>
+      </c>
+      <c r="G4" t="s">
+        <v>223</v>
+      </c>
+      <c r="H4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>285</v>
+      </c>
+      <c r="D5" s="1">
+        <v>7.24</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" ref="G5:G14" si="0">(E5-F5)*D5</f>
+        <v>14.48</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>286</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>287</v>
+      </c>
+      <c r="D6" s="1">
+        <v>7.7</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="0"/>
+        <v>15.4</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>308</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>313</v>
+      </c>
+      <c r="D7" s="1">
+        <v>24.95</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="0"/>
+        <v>49.9</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>312</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>320</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>306</v>
+      </c>
+      <c r="D9" s="1">
+        <v>49.95</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="0"/>
+        <v>199.8</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>371</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>372</v>
+      </c>
+      <c r="D11" s="1">
+        <v>52</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="0"/>
+        <v>104</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>304</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>309</v>
+      </c>
+      <c r="D12" s="1">
+        <v>21.99</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="0"/>
+        <v>21.99</v>
+      </c>
+      <c r="H12" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>329</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>321</v>
+      </c>
+      <c r="D13" s="1">
+        <v>12.94</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="0"/>
+        <v>25.88</v>
+      </c>
+      <c r="H13" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>290</v>
+      </c>
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14" t="s">
+        <v>310</v>
+      </c>
+      <c r="D14" s="1">
+        <v>6.04</v>
+      </c>
+      <c r="E14">
+        <v>8</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="0"/>
+        <v>48.32</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G15" s="1">
+        <f>SUM(G5:G14)</f>
+        <v>479.77000000000004</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H9" r:id="rId1" xr:uid="{D015C5EB-6B16-0744-8964-924D048D7799}"/>
+    <hyperlink ref="H7" r:id="rId2" xr:uid="{87546791-3990-2846-B60F-64D77FF64AB4}"/>
+    <hyperlink ref="H14" r:id="rId3" xr:uid="{8FEB2D40-243D-EB40-9049-84074FF0142B}"/>
+    <hyperlink ref="H11" r:id="rId4" xr:uid="{22360F0A-D1DC-4044-BB99-A5169A06BF1F}"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L130"/>
   <sheetViews>
@@ -3627,36 +4234,36 @@
       <selection activeCell="L74" sqref="L74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
     <col min="2" max="2" width="62" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="7.625" customWidth="1"/>
+    <col min="4" max="4" width="18.625" customWidth="1"/>
     <col min="5" max="5" width="11.5" customWidth="1"/>
     <col min="6" max="6" width="13.5" customWidth="1"/>
     <col min="7" max="8" width="11" customWidth="1"/>
     <col min="9" max="9" width="12.5" customWidth="1"/>
-    <col min="10" max="10" width="16.1640625" customWidth="1"/>
-    <col min="11" max="11" width="18.1640625" customWidth="1"/>
+    <col min="10" max="10" width="16.125" customWidth="1"/>
+    <col min="11" max="11" width="18.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -3694,7 +4301,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -3732,7 +4339,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -3767,7 +4374,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -3802,7 +4409,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -3837,7 +4444,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>8</v>
       </c>
@@ -3872,7 +4479,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>9</v>
       </c>
@@ -3910,7 +4517,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -3948,7 +4555,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -3983,7 +4590,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>12</v>
       </c>
@@ -4018,7 +4625,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>13</v>
       </c>
@@ -4053,7 +4660,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>14</v>
       </c>
@@ -4088,7 +4695,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>15</v>
       </c>
@@ -4123,7 +4730,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>16</v>
       </c>
@@ -4158,7 +4765,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>17</v>
       </c>
@@ -4193,7 +4800,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>18</v>
       </c>
@@ -4228,7 +4835,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>19</v>
       </c>
@@ -4263,7 +4870,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>20</v>
       </c>
@@ -4298,7 +4905,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>21</v>
       </c>
@@ -4333,7 +4940,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>22</v>
       </c>
@@ -4368,7 +4975,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>23</v>
       </c>
@@ -4406,7 +5013,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>24</v>
       </c>
@@ -4444,7 +5051,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>25</v>
       </c>
@@ -4479,7 +5086,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>26</v>
       </c>
@@ -4517,7 +5124,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>27</v>
       </c>
@@ -4555,7 +5162,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -4596,7 +5203,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>30</v>
       </c>
@@ -4634,7 +5241,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>31</v>
       </c>
@@ -4672,7 +5279,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>32</v>
       </c>
@@ -4710,7 +5317,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>33</v>
       </c>
@@ -4745,7 +5352,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>34</v>
       </c>
@@ -4783,7 +5390,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>35</v>
       </c>
@@ -4821,7 +5428,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>36</v>
       </c>
@@ -4859,7 +5466,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>263</v>
       </c>
@@ -4894,7 +5501,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>264</v>
       </c>
@@ -4929,7 +5536,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>37</v>
       </c>
@@ -4967,7 +5574,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>265</v>
       </c>
@@ -5005,7 +5612,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>38</v>
       </c>
@@ -5040,7 +5647,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>39</v>
       </c>
@@ -5078,7 +5685,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>267</v>
       </c>
@@ -5113,7 +5720,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>40</v>
       </c>
@@ -5151,7 +5758,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>41</v>
       </c>
@@ -5189,7 +5796,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>42</v>
       </c>
@@ -5227,7 +5834,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>44</v>
       </c>
@@ -5262,7 +5869,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>45</v>
       </c>
@@ -5288,7 +5895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>46</v>
       </c>
@@ -5326,7 +5933,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>47</v>
       </c>
@@ -5361,7 +5968,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>48</v>
       </c>
@@ -5399,7 +6006,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>49</v>
       </c>
@@ -5434,7 +6041,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>235</v>
       </c>
@@ -5472,7 +6079,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>234</v>
       </c>
@@ -5510,7 +6117,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>238</v>
       </c>
@@ -5548,7 +6155,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>239</v>
       </c>
@@ -5586,7 +6193,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>50</v>
       </c>
@@ -5624,7 +6231,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>51</v>
       </c>
@@ -5662,7 +6269,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>52</v>
       </c>
@@ -5700,7 +6307,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>243</v>
       </c>
@@ -5738,7 +6345,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>53</v>
       </c>
@@ -5776,7 +6383,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>54</v>
       </c>
@@ -5814,7 +6421,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>55</v>
       </c>
@@ -5849,7 +6456,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>56</v>
       </c>
@@ -5884,7 +6491,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>57</v>
       </c>
@@ -5919,7 +6526,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>58</v>
       </c>
@@ -5954,7 +6561,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>59</v>
       </c>
@@ -5989,7 +6596,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>60</v>
       </c>
@@ -6024,7 +6631,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>61</v>
       </c>
@@ -6062,7 +6669,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>62</v>
       </c>
@@ -6100,7 +6707,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>232</v>
       </c>
@@ -6136,7 +6743,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>63</v>
       </c>
@@ -6177,7 +6784,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>64</v>
       </c>
@@ -6215,7 +6822,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>66</v>
       </c>
@@ -6250,7 +6857,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>67</v>
       </c>
@@ -6288,7 +6895,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>68</v>
       </c>
@@ -6323,7 +6930,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>69</v>
       </c>
@@ -6358,7 +6965,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>70</v>
       </c>
@@ -6393,7 +7000,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>274</v>
       </c>
@@ -6428,7 +7035,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>71</v>
       </c>
@@ -6469,7 +7076,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>73</v>
       </c>
@@ -6504,7 +7111,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>74</v>
       </c>
@@ -6539,7 +7146,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>227</v>
       </c>
@@ -6574,7 +7181,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>75</v>
       </c>
@@ -6609,7 +7216,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>76</v>
       </c>
@@ -6647,7 +7254,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>77</v>
       </c>
@@ -6673,7 +7280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>275</v>
       </c>
@@ -6699,7 +7306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>78</v>
       </c>
@@ -6737,7 +7344,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>79</v>
       </c>
@@ -6775,7 +7382,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>80</v>
       </c>
@@ -6816,7 +7423,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>81</v>
       </c>
@@ -6851,7 +7458,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>82</v>
       </c>
@@ -6889,7 +7496,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>83</v>
       </c>
@@ -6927,7 +7534,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>110</v>
       </c>
@@ -6953,7 +7560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>111</v>
       </c>
@@ -6979,7 +7586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>112</v>
       </c>
@@ -7005,7 +7612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>113</v>
       </c>
@@ -7031,7 +7638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>84</v>
       </c>
@@ -7057,7 +7664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>85</v>
       </c>
@@ -7083,7 +7690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>296</v>
       </c>
@@ -7121,7 +7728,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="102" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>96</v>
       </c>
@@ -7159,7 +7766,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="103" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>292</v>
       </c>
@@ -7197,7 +7804,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="104" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>86</v>
       </c>
@@ -7232,7 +7839,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="105" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>87</v>
       </c>
@@ -7267,7 +7874,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="106" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>88</v>
       </c>
@@ -7302,7 +7909,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="107" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>89</v>
       </c>
@@ -7337,7 +7944,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="108" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>90</v>
       </c>
@@ -7372,7 +7979,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="109" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>91</v>
       </c>
@@ -7407,7 +8014,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="110" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>92</v>
       </c>
@@ -7442,7 +8049,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="111" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>93</v>
       </c>
@@ -7477,7 +8084,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="112" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>94</v>
       </c>
@@ -7512,7 +8119,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>95</v>
       </c>
@@ -7547,7 +8154,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>97</v>
       </c>
@@ -7582,7 +8189,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>96</v>
       </c>
@@ -7617,7 +8224,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>98</v>
       </c>
@@ -7655,7 +8262,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>99</v>
       </c>
@@ -7693,7 +8300,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>100</v>
       </c>
@@ -7728,7 +8335,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>276</v>
       </c>
@@ -7766,7 +8373,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>101</v>
       </c>
@@ -7801,7 +8408,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>102</v>
       </c>
@@ -7838,7 +8445,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
         <v>231</v>
       </c>
@@ -7868,7 +8475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>269</v>
       </c>
@@ -7906,7 +8513,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>270</v>
       </c>
@@ -7936,7 +8543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>271</v>
       </c>
@@ -7966,7 +8573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>103</v>
       </c>
@@ -8004,7 +8611,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>105</v>
       </c>
@@ -8030,7 +8637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>106</v>
       </c>
@@ -8068,7 +8675,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="129" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>107</v>
       </c>
@@ -8106,7 +8713,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="130" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:12" x14ac:dyDescent="0.25">
       <c r="I130" s="1">
         <f>SUM(I6:I129)</f>
         <v>1446.1700000000003</v>

</xml_diff>

<commit_message>
Updates BOM with dragon burner toolhead links.
</commit_message>
<xml_diff>
--- a/BOM/voron_2_tall_bom.xlsx
+++ b/BOM/voron_2_tall_bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ppak1\GitHub\Voron-2-Tall\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1783CE05-B7B8-42AB-9B6B-733527D24DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A36C81-56D9-40F8-9FB0-3C46347A3761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1_custom_kit" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="437">
   <si>
     <t>Category</t>
   </si>
@@ -1167,9 +1167,6 @@
     <t>Necessary Materials</t>
   </si>
   <si>
-    <t>Option 2: Canbus</t>
-  </si>
-  <si>
     <t>1. LDO Kit + Custom Materials</t>
   </si>
   <si>
@@ -1222,6 +1219,135 @@
   </si>
   <si>
     <t>Pack of 100</t>
+  </si>
+  <si>
+    <t>2. Dragon Burner V8 2.85mm Filament Toolhead</t>
+  </si>
+  <si>
+    <t>Big Tree Tech EBB SB2209</t>
+  </si>
+  <si>
+    <t>https://biqu.equipment/products/bigtreetech-ebb-sb2209-can-v1-0</t>
+  </si>
+  <si>
+    <t>For Stealthburner</t>
+  </si>
+  <si>
+    <t>https://biqu.equipment/products/bigtreetech-ebb-sb2209-can-v1-0?variant=40214284468322</t>
+  </si>
+  <si>
+    <t>U2C V2.1</t>
+  </si>
+  <si>
+    <t>https://biqu.equipment/products/bigtreetech-ebb-sb2209-can-v1-0?variant=40214285058146</t>
+  </si>
+  <si>
+    <t>30 PIN Wire + 100K NTC B3950</t>
+  </si>
+  <si>
+    <t>Can use RJ11 port on Octopus instead</t>
+  </si>
+  <si>
+    <t>Precrimped small wires (recommended)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B098NKKZ3B?psc=1&amp;ref=ppx_yo2ov_dt_b_product_details</t>
+  </si>
+  <si>
+    <t>Aesthetic covering for canbus wire</t>
+  </si>
+  <si>
+    <t>25ft - 1/4 inch PET Expandable Braided Sleeving</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B09Z26FF8B?ref=ppx_yo2ov_dt_b_product_details&amp;th=1</t>
+  </si>
+  <si>
+    <t>PG7 is used</t>
+  </si>
+  <si>
+    <t>Cable Connectors PG7 PG9 PG11 PG13.5 PG16 PG19</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B0CNXRZTKL?psc=1&amp;ref=ppx_yo2ov_dt_b_product_details</t>
+  </si>
+  <si>
+    <t>Big Tree Tech EBB36</t>
+  </si>
+  <si>
+    <t>Alternative canbus PCB</t>
+  </si>
+  <si>
+    <t>22 AWG Black and Red Silicone Wire</t>
+  </si>
+  <si>
+    <t>Delivers power to PCB</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B077XBWX8V/ref=ppx_yo_dt_b_asin_title_o00_s00?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B0CWP24SL5/ref=ppx_yo_dt_b_asin_title_o00_s00?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>Ferrule Crimping Tool AWG 23-7 with 1900PCS Ferrules Kit</t>
+  </si>
+  <si>
+    <t>Crimping for hotend wiring</t>
+  </si>
+  <si>
+    <t>https://e3d-online.com/products/v6-all-metal-hotend?variant=40923457519675</t>
+  </si>
+  <si>
+    <t>V6 All-Metal HotEnd</t>
+  </si>
+  <si>
+    <t>2.85mm 24V Direct Drive</t>
+  </si>
+  <si>
+    <t>FYSETC Sequins with RGB WS2812 3535 Bright RGB LED</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.us/item/3256805836898589.html?spm=a2g0o.order_list.order_list_main.5.be2c1802BzLH1m&amp;gatewayAdapt=glo2usa</t>
+  </si>
+  <si>
+    <t>Pack of 2</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.us/item/3256802670785330.html?spm=a2g0o.order_detail.order_detail_item.3.71e0f19chbGpOS&amp;gatewayAdapt=glo2usa</t>
+  </si>
+  <si>
+    <t>40 x 40 x 10 mm Brushless Exhaust Cooler Printer Radiators</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.us/item/2251832613009306.html?spm=a2g0o.order_detail.order_detail_item.5.71e0f19chbGpOS&amp;gatewayAdapt=glo2usa</t>
+  </si>
+  <si>
+    <t>Side fans for cowl</t>
+  </si>
+  <si>
+    <t>30 x 30 x 10 mm Dual Ball Bearing Brushless Car Lamp Cooling Fan</t>
+  </si>
+  <si>
+    <t>Rainbow RGBW LEDs</t>
+  </si>
+  <si>
+    <t>Rainbow Barf</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.us/item/3256805225841575.html?spm=a2g0o.order_detail.order_detail_item.3.685df19cPUQqF7&amp;gatewayAdapt=glo2usa</t>
+  </si>
+  <si>
+    <t>Orbiter Extruder for 2.85/3.0MM Filament</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.us/item/3256802594760158.html?spm=a2g0o.order_list.order_list_main.29.be2c1802BzLH1m&amp;gatewayAdapt=glo2usa</t>
+  </si>
+  <si>
+    <t>Provided fully assembled</t>
+  </si>
+  <si>
+    <t>Extra (60) Chain Links for height</t>
   </si>
 </sst>
 </file>
@@ -1769,7 +1895,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
@@ -1784,7 +1910,6 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="8" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2143,8 +2268,1326 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F651F1D0-7A81-0546-9600-A8B0A78885C7}">
   <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="57.5" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="34.375" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="7.375" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="10.375" customWidth="1"/>
+    <col min="8" max="8" width="9.875" customWidth="1"/>
+    <col min="9" max="9" width="10.375" customWidth="1"/>
+    <col min="10" max="10" width="18.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="6" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E4" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="H4" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="I4" s="11"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="G5" t="s">
+        <v>366</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>386</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>387</v>
+      </c>
+      <c r="J5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>299</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>300</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1449</v>
+      </c>
+      <c r="E6" s="7">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <f>F6*D6</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="12">
+        <f xml:space="preserve"> D6*E6</f>
+        <v>1449</v>
+      </c>
+      <c r="I6" s="12">
+        <f t="shared" ref="I6:I10" si="0">(E6-F6)*D6</f>
+        <v>1449</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>369</v>
+      </c>
+      <c r="B7">
+        <v>100</v>
+      </c>
+      <c r="C7" t="s">
+        <v>393</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5.99</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="12">
+        <f t="shared" ref="H7:H15" si="1" xml:space="preserve"> D7*E7</f>
+        <v>5.99</v>
+      </c>
+      <c r="I7" s="12">
+        <f t="shared" si="0"/>
+        <v>5.99</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <v>163</v>
+      </c>
+      <c r="C8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" s="1">
+        <v>12.88</v>
+      </c>
+      <c r="E8" s="7">
+        <v>2</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" ref="G8:G16" si="2">F8*D8</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="12">
+        <f t="shared" si="1"/>
+        <v>25.76</v>
+      </c>
+      <c r="I8" s="12">
+        <f t="shared" si="0"/>
+        <v>25.76</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>302</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>303</v>
+      </c>
+      <c r="D9" s="1">
+        <v>30.91</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="12">
+        <f t="shared" si="1"/>
+        <v>30.91</v>
+      </c>
+      <c r="I9" s="12">
+        <f t="shared" si="0"/>
+        <v>30.91</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>267</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="D10" s="3">
+        <v>66</v>
+      </c>
+      <c r="E10" s="7">
+        <v>4</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="12">
+        <f t="shared" si="1"/>
+        <v>264</v>
+      </c>
+      <c r="I10" s="12">
+        <f t="shared" si="0"/>
+        <v>264</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>274</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>279</v>
+      </c>
+      <c r="D11" s="1">
+        <v>25.97</v>
+      </c>
+      <c r="E11" s="7">
+        <v>4</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="12">
+        <f t="shared" si="1"/>
+        <v>103.88</v>
+      </c>
+      <c r="I11" s="12">
+        <f t="shared" ref="I11" si="3">(E11-F11)*D11</f>
+        <v>103.88</v>
+      </c>
+      <c r="J11" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>281</v>
+      </c>
+      <c r="D12" s="1">
+        <v>8.99</v>
+      </c>
+      <c r="E12" s="7">
+        <v>1</v>
+      </c>
+      <c r="F12" s="7">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="12">
+        <f t="shared" si="1"/>
+        <v>8.99</v>
+      </c>
+      <c r="I12" s="12">
+        <f>(E12-F12)*D12</f>
+        <v>8.99</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>276</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>436</v>
+      </c>
+      <c r="D13" s="1">
+        <v>46.44</v>
+      </c>
+      <c r="E13" s="7">
+        <v>1</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="12">
+        <f t="shared" si="1"/>
+        <v>46.44</v>
+      </c>
+      <c r="I13" s="12">
+        <f t="shared" ref="I13:I15" si="4">(E13-F13)*D13</f>
+        <v>46.44</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>101</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>6.12</v>
+      </c>
+      <c r="E14" s="7">
+        <v>1</v>
+      </c>
+      <c r="F14" s="7">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="12">
+        <f t="shared" si="1"/>
+        <v>6.12</v>
+      </c>
+      <c r="I14" s="12">
+        <f t="shared" si="4"/>
+        <v>6.12</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>316</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>314</v>
+      </c>
+      <c r="D15" s="1">
+        <v>139.80000000000001</v>
+      </c>
+      <c r="E15" s="7">
+        <v>1</v>
+      </c>
+      <c r="F15" s="7">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="12">
+        <f t="shared" si="1"/>
+        <v>139.80000000000001</v>
+      </c>
+      <c r="I15" s="12">
+        <f t="shared" si="4"/>
+        <v>139.80000000000001</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>315</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="1"/>
+      <c r="G17" s="1">
+        <f>SUM(G6:G16)</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <f>SUM(H6:H16)</f>
+        <v>2080.89</v>
+      </c>
+      <c r="I17" s="1">
+        <f>SUM(I6:I16)</f>
+        <v>2080.89</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J10" r:id="rId1" xr:uid="{B069B4F7-3B34-1F4D-91FE-BAFC3C3AFDEB}"/>
+    <hyperlink ref="J9" r:id="rId2" xr:uid="{A674AA42-7047-D742-B0B0-F79013D37D21}"/>
+    <hyperlink ref="J15" r:id="rId3" xr:uid="{933BC923-64A5-364D-B1D1-AA0CD0F86FE7}"/>
+    <hyperlink ref="J14" r:id="rId4" xr:uid="{040C449F-BD13-3A40-A3CF-B6CEB04C54CC}"/>
+    <hyperlink ref="J13" r:id="rId5" xr:uid="{1BE03111-1688-3547-8700-06A03759C772}"/>
+    <hyperlink ref="J6" r:id="rId6" xr:uid="{95771CD4-335F-4BC9-AC44-BA0B6FF377F1}"/>
+    <hyperlink ref="J12" r:id="rId7" xr:uid="{9C5256D3-4225-4D6A-9A4B-B2579A49D423}"/>
+    <hyperlink ref="J8" r:id="rId8" display="https://www.aliexpress.us/item/2251832618848960.html?aff_fcid=8983d09608854cd680a9aafef2bc2e52-1700531331137-02956-KUHCwnu4&amp;aff_fsk=KUHCwnu4&amp;aff_platform=link-c-tool&amp;sk=KUHCwnu4&amp;aff_trace_key=8983d09608854cd680a9aafef2bc2e52-1700531331137-02956-KUHCwnu4&amp;terminal_id=77b480c9601746d1be2247846d74a043&amp;gatewayAdapt=glo2usa4itemAdapt" xr:uid="{A5526E6D-3905-46C5-80E0-4955235EDD02}"/>
+    <hyperlink ref="J7" r:id="rId9" xr:uid="{61D7288E-4A70-496D-8A5D-BB1863824592}"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B333F01F-4973-487B-89AC-950BB7EE7FAF}">
+  <dimension ref="A1:J55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="57.5" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="34.375" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="7.375" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="10.375" customWidth="1"/>
+    <col min="8" max="8" width="9.875" customWidth="1"/>
+    <col min="9" max="9" width="10.375" customWidth="1"/>
+    <col min="10" max="10" width="18.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>375</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="H6" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="I6" s="11"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>254</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="G7" t="s">
+        <v>366</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>386</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>387</v>
+      </c>
+      <c r="J7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>326</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>328</v>
+      </c>
+      <c r="D8" s="1">
+        <v>12.99</v>
+      </c>
+      <c r="E8" s="7">
+        <v>2</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" ref="G8:G9" si="0">F8*D8</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="12">
+        <f>D8*E8</f>
+        <v>25.98</v>
+      </c>
+      <c r="I8" s="12">
+        <f t="shared" ref="I8:I9" si="1">(E8-F8)*D8</f>
+        <v>25.98</v>
+      </c>
+      <c r="J8" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>346</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>347</v>
+      </c>
+      <c r="D9" s="1">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="12">
+        <f>D9*E9</f>
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="I9" s="12">
+        <f t="shared" si="1"/>
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D10" s="1"/>
+      <c r="G10" s="1">
+        <f>SUM(G8:G9)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <f>SUM(H8:H9)</f>
+        <v>35.93</v>
+      </c>
+      <c r="I10" s="1">
+        <f>SUM(I8:I9)</f>
+        <v>35.93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
+        <v>373</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="H12" s="10" t="s">
+        <v>361</v>
+      </c>
+      <c r="I12" s="11"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>254</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="G13" t="s">
+        <v>366</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>362</v>
+      </c>
+      <c r="J13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>294</v>
+      </c>
+      <c r="D14" s="1">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="E14" s="7">
+        <v>100</v>
+      </c>
+      <c r="F14" s="7">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" ref="G14:G23" si="2">F14*D14</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="12">
+        <f>D14*E14</f>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="I14" s="12">
+        <f t="shared" ref="I14:I23" si="3">(E14-F14)*D14</f>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="J14" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>292</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>293</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1.02</v>
+      </c>
+      <c r="E15" s="7">
+        <v>2</v>
+      </c>
+      <c r="F15" s="7">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="12">
+        <f t="shared" ref="H15:H23" si="4">D15*E15</f>
+        <v>2.04</v>
+      </c>
+      <c r="I15" s="12">
+        <f t="shared" si="3"/>
+        <v>2.04</v>
+      </c>
+      <c r="J15" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>334</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>332</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="E16" s="7">
+        <v>2</v>
+      </c>
+      <c r="F16" s="7">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="12">
+        <f t="shared" si="4"/>
+        <v>0.76</v>
+      </c>
+      <c r="I16" s="12">
+        <f t="shared" si="3"/>
+        <v>0.76</v>
+      </c>
+      <c r="J16" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>335</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>333</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="E17" s="7">
+        <v>2</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="12">
+        <f t="shared" si="4"/>
+        <v>0.8</v>
+      </c>
+      <c r="I17" s="12">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>337</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>338</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="E18" s="7">
+        <v>2</v>
+      </c>
+      <c r="F18" s="7">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="12">
+        <f t="shared" si="4"/>
+        <v>1.72</v>
+      </c>
+      <c r="I18" s="12">
+        <f t="shared" si="3"/>
+        <v>1.72</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>354</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>355</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1.02</v>
+      </c>
+      <c r="E19" s="7">
+        <v>2</v>
+      </c>
+      <c r="F19" s="7">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="12">
+        <f t="shared" si="4"/>
+        <v>2.04</v>
+      </c>
+      <c r="I19" s="12">
+        <f t="shared" si="3"/>
+        <v>2.04</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>340</v>
+      </c>
+      <c r="B20">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>343</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.122</v>
+      </c>
+      <c r="E20" s="7">
+        <v>100</v>
+      </c>
+      <c r="F20" s="7">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="12">
+        <f t="shared" si="4"/>
+        <v>12.2</v>
+      </c>
+      <c r="I20" s="12">
+        <f t="shared" si="3"/>
+        <v>12.2</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>342</v>
+      </c>
+      <c r="B21">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
+        <v>344</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.114</v>
+      </c>
+      <c r="E21" s="7">
+        <v>100</v>
+      </c>
+      <c r="F21" s="7">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="12">
+        <f t="shared" si="4"/>
+        <v>11.4</v>
+      </c>
+      <c r="I21" s="12">
+        <f t="shared" si="3"/>
+        <v>11.4</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>356</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>357</v>
+      </c>
+      <c r="D22" s="1">
+        <v>89.54</v>
+      </c>
+      <c r="E22" s="7">
+        <v>1</v>
+      </c>
+      <c r="F22" s="7">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="12">
+        <f t="shared" si="4"/>
+        <v>89.54</v>
+      </c>
+      <c r="I22" s="12">
+        <f t="shared" si="3"/>
+        <v>89.54</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>352</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>353</v>
+      </c>
+      <c r="D23" s="1">
+        <v>8.9</v>
+      </c>
+      <c r="E23" s="7">
+        <v>1</v>
+      </c>
+      <c r="F23" s="7">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="12">
+        <f t="shared" si="4"/>
+        <v>8.9</v>
+      </c>
+      <c r="I23" s="12">
+        <f t="shared" si="3"/>
+        <v>8.9</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G24" s="1">
+        <f>SUM(G14:G23)</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="1">
+        <f>SUM(H14:H23)</f>
+        <v>137.70000000000002</v>
+      </c>
+      <c r="I24" s="1">
+        <f>SUM(I14:I23)</f>
+        <v>137.70000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>374</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="F26" s="9"/>
+      <c r="H26" s="10" t="s">
+        <v>361</v>
+      </c>
+      <c r="I26" s="11"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>254</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>114</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="G27" t="s">
+        <v>366</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>362</v>
+      </c>
+      <c r="J27" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>395</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>397</v>
+      </c>
+      <c r="D28" s="1">
+        <v>39.99</v>
+      </c>
+      <c r="E28" s="7">
+        <v>1</v>
+      </c>
+      <c r="F28" s="7">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1">
+        <f t="shared" ref="G28:G32" si="5">F28*D28</f>
+        <v>0</v>
+      </c>
+      <c r="H28" s="12">
+        <f>D28*E28</f>
+        <v>39.99</v>
+      </c>
+      <c r="I28" s="12">
+        <f t="shared" ref="I28:I32" si="6">(E28-F28)*D28</f>
+        <v>39.99</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>399</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29" t="s">
+        <v>402</v>
+      </c>
+      <c r="D29" s="1">
+        <v>46.88</v>
+      </c>
+      <c r="E29" s="7">
+        <v>1</v>
+      </c>
+      <c r="F29" s="7">
+        <v>0</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="12">
+        <f t="shared" ref="H29:H32" si="7">D29*E29</f>
+        <v>46.88</v>
+      </c>
+      <c r="I29" s="12">
+        <f t="shared" si="6"/>
+        <v>46.88</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>401</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>403</v>
+      </c>
+      <c r="D30" s="1">
+        <v>6.55</v>
+      </c>
+      <c r="E30" s="7">
+        <v>1</v>
+      </c>
+      <c r="F30" s="7">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="12">
+        <f t="shared" si="7"/>
+        <v>6.55</v>
+      </c>
+      <c r="I30" s="12">
+        <f t="shared" si="6"/>
+        <v>6.55</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>406</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>405</v>
+      </c>
+      <c r="D31" s="1">
+        <v>8.99</v>
+      </c>
+      <c r="E31" s="7">
+        <v>1</v>
+      </c>
+      <c r="F31" s="7">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H31" s="12">
+        <f t="shared" si="7"/>
+        <v>8.99</v>
+      </c>
+      <c r="I31" s="12">
+        <f t="shared" si="6"/>
+        <v>8.99</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>409</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>408</v>
+      </c>
+      <c r="D32" s="1">
+        <v>12.99</v>
+      </c>
+      <c r="E32" s="7">
+        <v>1</v>
+      </c>
+      <c r="F32" s="7">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="12">
+        <f t="shared" si="7"/>
+        <v>12.99</v>
+      </c>
+      <c r="I32" s="12">
+        <f t="shared" si="6"/>
+        <v>12.99</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="33" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G33" s="1">
+        <f>SUM(G28:G32)</f>
+        <v>0</v>
+      </c>
+      <c r="H33" s="1">
+        <f>SUM(H28:H32)</f>
+        <v>115.39999999999999</v>
+      </c>
+      <c r="I33" s="1">
+        <f>SUM(I28:I32)</f>
+        <v>115.39999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J17" r:id="rId1" xr:uid="{8F88ED9B-1C89-4651-AF81-0D0D1136F20A}"/>
+    <hyperlink ref="J28" r:id="rId2" xr:uid="{4A427926-25AE-408E-8933-96E771F0BC6A}"/>
+    <hyperlink ref="J29" r:id="rId3" xr:uid="{9F180175-614F-435C-92C8-060EB21E1DCD}"/>
+    <hyperlink ref="J30" r:id="rId4" xr:uid="{CF04AA44-1000-4E51-A205-6D3DCCB678FD}"/>
+    <hyperlink ref="J32" r:id="rId5" xr:uid="{1FF6EA14-C717-49A5-BB0F-777905E1FD54}"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId6"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{645409AD-79BA-4214-8D29-3BF242B131B1}">
+  <dimension ref="A1:J68"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2173,98 +3616,66 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E4" s="8" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>381</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>363</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="H4" s="10" t="s">
-        <v>389</v>
-      </c>
-      <c r="I4" s="11"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>254</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>114</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>364</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>365</v>
-      </c>
-      <c r="G5" t="s">
-        <v>366</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>387</v>
-      </c>
-      <c r="I5" s="11" t="s">
+      <c r="F5" s="9"/>
+      <c r="H5" s="10" t="s">
         <v>388</v>
       </c>
-      <c r="J5" t="s">
-        <v>115</v>
-      </c>
+      <c r="I5" s="11"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>299</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>254</v>
       </c>
       <c r="C6" t="s">
-        <v>300</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1449</v>
-      </c>
-      <c r="E6" s="7">
-        <v>1</v>
-      </c>
-      <c r="F6" s="7">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1">
-        <f>F6*D6</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="12">
-        <f xml:space="preserve"> D6*E6</f>
-        <v>1449</v>
-      </c>
-      <c r="I6" s="12">
-        <f t="shared" ref="I6:I10" si="0">(E6-F6)*D6</f>
-        <v>1449</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>301</v>
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="G6" t="s">
+        <v>366</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>386</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>387</v>
+      </c>
+      <c r="J6" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>369</v>
+        <v>382</v>
       </c>
       <c r="B7">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="D7" s="1">
-        <v>5.99</v>
+        <v>80</v>
       </c>
       <c r="E7" s="7">
         <v>1</v>
@@ -2273,67 +3684,68 @@
         <v>0</v>
       </c>
       <c r="G7" s="1">
+        <f>F7*D7</f>
         <v>0</v>
       </c>
       <c r="H7" s="12">
-        <f t="shared" ref="H7:H15" si="1" xml:space="preserve"> D7*E7</f>
-        <v>5.99</v>
+        <f>D7*E7</f>
+        <v>80</v>
       </c>
       <c r="I7" s="12">
-        <f t="shared" si="0"/>
-        <v>5.99</v>
-      </c>
-      <c r="J7" t="s">
-        <v>368</v>
+        <f>(E7-F7)*D7</f>
+        <v>80</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>384</v>
       </c>
       <c r="B8">
-        <v>163</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>137</v>
+        <v>390</v>
       </c>
       <c r="D8" s="1">
-        <v>12.88</v>
+        <v>5</v>
       </c>
       <c r="E8" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" s="7">
         <v>0</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" ref="G8:G16" si="2">F8*D8</f>
+        <f>F8*D8</f>
         <v>0</v>
       </c>
       <c r="H8" s="12">
-        <f t="shared" si="1"/>
-        <v>25.76</v>
+        <f>D8*E8</f>
+        <v>5</v>
       </c>
       <c r="I8" s="12">
-        <f t="shared" si="0"/>
-        <v>25.76</v>
-      </c>
-      <c r="J8" t="s">
-        <v>138</v>
+        <f>(E8-F8)*D8</f>
+        <v>5</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>302</v>
+        <v>324</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>303</v>
+        <v>325</v>
       </c>
       <c r="D9" s="1">
-        <v>30.91</v>
+        <v>15.99</v>
       </c>
       <c r="E9" s="7">
         <v>1</v>
@@ -2342,252 +3754,479 @@
         <v>0</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" si="2"/>
+        <f>F9*D9</f>
         <v>0</v>
       </c>
       <c r="H9" s="12">
-        <f t="shared" si="1"/>
-        <v>30.91</v>
+        <f t="shared" ref="H9:H11" si="0">D9*E9</f>
+        <v>15.99</v>
       </c>
       <c r="I9" s="12">
-        <f t="shared" si="0"/>
-        <v>30.91</v>
+        <f>(E9-F9)*D9</f>
+        <v>15.99</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>145</v>
+        <v>323</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>267</v>
+        <v>349</v>
       </c>
       <c r="B10">
-        <v>4</v>
-      </c>
-      <c r="D10" s="3">
-        <v>66</v>
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>350</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
       </c>
       <c r="E10" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F10" s="7">
         <v>0</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" si="2"/>
+        <f>F10*D10</f>
         <v>0</v>
       </c>
       <c r="H10" s="12">
-        <f t="shared" si="1"/>
-        <v>264</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="I10" s="12">
-        <f t="shared" si="0"/>
-        <v>264</v>
+        <f>(E10-F10)*D10</f>
+        <v>1</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>268</v>
+        <v>348</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>274</v>
+        <v>359</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>279</v>
+        <v>391</v>
       </c>
       <c r="D11" s="1">
-        <v>25.97</v>
+        <v>14.36</v>
       </c>
       <c r="E11" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F11" s="7">
         <v>0</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" si="2"/>
+        <f>F11*D11</f>
         <v>0</v>
       </c>
       <c r="H11" s="12">
-        <f t="shared" si="1"/>
-        <v>103.88</v>
+        <f t="shared" si="0"/>
+        <v>14.36</v>
       </c>
       <c r="I11" s="12">
-        <f t="shared" ref="I11" si="3">(E11-F11)*D11</f>
-        <v>103.88</v>
-      </c>
-      <c r="J11" t="s">
-        <v>278</v>
+        <f>(E11-F11)*D11</f>
+        <v>14.36</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>281</v>
-      </c>
-      <c r="D12" s="1">
-        <v>8.99</v>
-      </c>
-      <c r="E12" s="7">
-        <v>1</v>
-      </c>
-      <c r="F12" s="7">
-        <v>0</v>
-      </c>
+      <c r="D12" s="1"/>
       <c r="G12" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H12" s="12">
-        <f t="shared" si="1"/>
-        <v>8.99</v>
-      </c>
-      <c r="I12" s="12">
-        <f>(E12-F12)*D12</f>
-        <v>8.99</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>276</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>277</v>
-      </c>
-      <c r="D13" s="1">
-        <v>46.44</v>
-      </c>
-      <c r="E13" s="7">
-        <v>1</v>
-      </c>
-      <c r="F13" s="7">
-        <v>0</v>
-      </c>
-      <c r="G13" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H13" s="12">
-        <f t="shared" si="1"/>
-        <v>46.44</v>
-      </c>
-      <c r="I13" s="12">
-        <f t="shared" ref="I13:I15" si="4">(E13-F13)*D13</f>
-        <v>46.44</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>217</v>
+        <f>SUM(G9:G11)</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <f>SUM(H7:H11)</f>
+        <v>116.35</v>
+      </c>
+      <c r="I12" s="1">
+        <f>SUM(I7:I11)</f>
+        <v>116.35</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>101</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1">
-        <v>6.12</v>
-      </c>
-      <c r="E14" s="7">
-        <v>1</v>
-      </c>
-      <c r="F14" s="7">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H14" s="12">
-        <f t="shared" si="1"/>
-        <v>6.12</v>
-      </c>
-      <c r="I14" s="12">
-        <f t="shared" si="4"/>
-        <v>6.12</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>217</v>
-      </c>
+      <c r="A14" s="13" t="s">
+        <v>394</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="H14" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="I14" s="11"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>316</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>254</v>
       </c>
       <c r="C15" t="s">
-        <v>314</v>
-      </c>
-      <c r="D15" s="1">
-        <v>139.80000000000001</v>
-      </c>
-      <c r="E15" s="7">
-        <v>1</v>
-      </c>
-      <c r="F15" s="7">
-        <v>0</v>
-      </c>
-      <c r="G15" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H15" s="12">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="G15" t="s">
+        <v>366</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>386</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>387</v>
+      </c>
+      <c r="J15" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>411</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>412</v>
+      </c>
+      <c r="D16" s="1">
+        <v>29.99</v>
+      </c>
+      <c r="E16" s="7">
+        <v>1</v>
+      </c>
+      <c r="F16" s="7">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <f>F16*D16</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="12">
+        <f>D16*E16</f>
+        <v>29.99</v>
+      </c>
+      <c r="I16" s="12">
+        <f>(E16-F16)*D16</f>
+        <v>29.99</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>413</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>414</v>
+      </c>
+      <c r="D17" s="1">
+        <v>9.98</v>
+      </c>
+      <c r="E17" s="7">
+        <v>1</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <f>F17*D17</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="12">
+        <f>D17*E17</f>
+        <v>9.98</v>
+      </c>
+      <c r="I17" s="12">
+        <f>(E17-F17)*D17</f>
+        <v>9.98</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>417</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>418</v>
+      </c>
+      <c r="D18" s="1">
+        <v>23.98</v>
+      </c>
+      <c r="E18" s="7">
+        <v>1</v>
+      </c>
+      <c r="F18" s="7">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <f>F18*D18</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="12">
+        <f t="shared" ref="H18:H24" si="1">D18*E18</f>
+        <v>23.98</v>
+      </c>
+      <c r="I18" s="12">
+        <f>(E18-F18)*D18</f>
+        <v>23.98</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>420</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>421</v>
+      </c>
+      <c r="D19" s="1">
+        <v>45.39</v>
+      </c>
+      <c r="E19" s="7">
+        <v>1</v>
+      </c>
+      <c r="F19" s="7">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <f>F19*D19</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="12">
         <f t="shared" si="1"/>
-        <v>139.80000000000001</v>
-      </c>
-      <c r="I15" s="12">
-        <f t="shared" si="4"/>
-        <v>139.80000000000001</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>315</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-    </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D17" s="1"/>
-      <c r="G17" s="1">
-        <f>SUM(G6:G16)</f>
-        <v>0</v>
-      </c>
-      <c r="H17" s="1">
-        <f>SUM(H6:H16)</f>
-        <v>2080.89</v>
-      </c>
-      <c r="I17" s="1">
-        <f>SUM(I6:I16)</f>
-        <v>2080.89</v>
+        <v>45.39</v>
+      </c>
+      <c r="I19" s="12">
+        <f>(E19-F19)*D19</f>
+        <v>45.39</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>426</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>428</v>
+      </c>
+      <c r="D20" s="1">
+        <v>5.93</v>
+      </c>
+      <c r="E20" s="7">
+        <v>2</v>
+      </c>
+      <c r="F20" s="7">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <f>F20*D20</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="12">
+        <f t="shared" si="1"/>
+        <v>11.86</v>
+      </c>
+      <c r="I20" s="12">
+        <f>(E20-F20)*D20</f>
+        <v>11.86</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>429</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>424</v>
+      </c>
+      <c r="D21" s="1">
+        <v>8.5399999999999991</v>
+      </c>
+      <c r="E21" s="7">
+        <v>1</v>
+      </c>
+      <c r="F21" s="7">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <f>F21*D21</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="12">
+        <f t="shared" si="1"/>
+        <v>8.5399999999999991</v>
+      </c>
+      <c r="I21" s="12">
+        <f>(E21-F21)*D21</f>
+        <v>8.5399999999999991</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>433</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>435</v>
+      </c>
+      <c r="D22" s="1">
+        <v>56.9</v>
+      </c>
+      <c r="E22" s="7">
+        <v>1</v>
+      </c>
+      <c r="F22" s="7">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
+        <f>F22*D22</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="12">
+        <f t="shared" si="1"/>
+        <v>56.9</v>
+      </c>
+      <c r="I22" s="12">
+        <f>(E22-F22)*D22</f>
+        <v>56.9</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>430</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>431</v>
+      </c>
+      <c r="D23" s="1">
+        <v>5.88</v>
+      </c>
+      <c r="E23" s="7">
+        <v>1</v>
+      </c>
+      <c r="F23" s="7">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1">
+        <f>F23*D23</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="12">
+        <f t="shared" si="1"/>
+        <v>5.88</v>
+      </c>
+      <c r="I23" s="12">
+        <f>(E23-F23)*D23</f>
+        <v>5.88</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>422</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>391</v>
+      </c>
+      <c r="D24" s="1">
+        <v>2.92</v>
+      </c>
+      <c r="E24" s="7">
+        <v>1</v>
+      </c>
+      <c r="F24" s="7">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1">
+        <f>F24*D24</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="12">
+        <f t="shared" si="1"/>
+        <v>2.92</v>
+      </c>
+      <c r="I24" s="12">
+        <f>(E24-F24)*D24</f>
+        <v>2.92</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D25" s="1"/>
+      <c r="G25" s="1">
+        <f>SUM(G18:G24)</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="1">
+        <f>SUM(H16:H24)</f>
+        <v>195.44</v>
+      </c>
+      <c r="I25" s="1">
+        <f>SUM(I16:I24)</f>
+        <v>195.44</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
@@ -2602,1313 +4241,13 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J10" r:id="rId1" xr:uid="{B069B4F7-3B34-1F4D-91FE-BAFC3C3AFDEB}"/>
-    <hyperlink ref="J9" r:id="rId2" xr:uid="{A674AA42-7047-D742-B0B0-F79013D37D21}"/>
-    <hyperlink ref="J15" r:id="rId3" xr:uid="{933BC923-64A5-364D-B1D1-AA0CD0F86FE7}"/>
-    <hyperlink ref="J14" r:id="rId4" xr:uid="{040C449F-BD13-3A40-A3CF-B6CEB04C54CC}"/>
-    <hyperlink ref="J13" r:id="rId5" xr:uid="{1BE03111-1688-3547-8700-06A03759C772}"/>
-    <hyperlink ref="J6" r:id="rId6" xr:uid="{95771CD4-335F-4BC9-AC44-BA0B6FF377F1}"/>
-    <hyperlink ref="J12" r:id="rId7" xr:uid="{9C5256D3-4225-4D6A-9A4B-B2579A49D423}"/>
-  </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B333F01F-4973-487B-89AC-950BB7EE7FAF}">
-  <dimension ref="A1:J60"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="57.5" customWidth="1"/>
-    <col min="2" max="2" width="10.5" customWidth="1"/>
-    <col min="3" max="3" width="34.375" customWidth="1"/>
-    <col min="4" max="4" width="11.5" customWidth="1"/>
-    <col min="5" max="5" width="7.375" customWidth="1"/>
-    <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="10.375" customWidth="1"/>
-    <col min="8" max="8" width="9.875" customWidth="1"/>
-    <col min="9" max="9" width="10.375" customWidth="1"/>
-    <col min="10" max="10" width="18.125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="6" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>375</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>363</v>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="H6" s="10" t="s">
-        <v>389</v>
-      </c>
-      <c r="I6" s="11"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>254</v>
-      </c>
-      <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>114</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>364</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>365</v>
-      </c>
-      <c r="G7" t="s">
-        <v>366</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>387</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>388</v>
-      </c>
-      <c r="J7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>326</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>328</v>
-      </c>
-      <c r="D8" s="1">
-        <v>12.99</v>
-      </c>
-      <c r="E8" s="7">
-        <v>2</v>
-      </c>
-      <c r="F8" s="7">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1">
-        <f t="shared" ref="G8:G9" si="0">F8*D8</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="12">
-        <f>D8*E8</f>
-        <v>25.98</v>
-      </c>
-      <c r="I8" s="12">
-        <f t="shared" ref="I8:I9" si="1">(E8-F8)*D8</f>
-        <v>25.98</v>
-      </c>
-      <c r="J8" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>346</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>347</v>
-      </c>
-      <c r="D9" s="1">
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="E9" s="7">
-        <v>1</v>
-      </c>
-      <c r="F9" s="7">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H9" s="12">
-        <f>D9*E9</f>
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="I9" s="12">
-        <f t="shared" si="1"/>
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D10" s="1"/>
-      <c r="G10" s="1">
-        <f>SUM(G8:G9)</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="1">
-        <f>SUM(H8:H9)</f>
-        <v>35.93</v>
-      </c>
-      <c r="I10" s="1">
-        <f>SUM(I8:I9)</f>
-        <v>35.93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>373</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>363</v>
-      </c>
-      <c r="F12" s="9"/>
-      <c r="H12" s="10" t="s">
-        <v>361</v>
-      </c>
-      <c r="I12" s="11"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>254</v>
-      </c>
-      <c r="C13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>114</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>364</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>365</v>
-      </c>
-      <c r="G13" t="s">
-        <v>366</v>
-      </c>
-      <c r="H13" s="11" t="s">
-        <v>360</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>362</v>
-      </c>
-      <c r="J13" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>96</v>
-      </c>
-      <c r="B14">
-        <v>28</v>
-      </c>
-      <c r="C14" t="s">
-        <v>294</v>
-      </c>
-      <c r="D14" s="1">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="E14" s="7">
-        <v>100</v>
-      </c>
-      <c r="F14" s="7">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1">
-        <f>F14*D14</f>
-        <v>0</v>
-      </c>
-      <c r="H14" s="12">
-        <f>D14*E14</f>
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="I14" s="12">
-        <f>(E14-F14)*D14</f>
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="J14" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>292</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>293</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1.02</v>
-      </c>
-      <c r="E15" s="7">
-        <v>2</v>
-      </c>
-      <c r="F15" s="7">
-        <v>0</v>
-      </c>
-      <c r="G15" s="1">
-        <f>F15*D15</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="12">
-        <f t="shared" ref="H15:H23" si="2">D15*E15</f>
-        <v>2.04</v>
-      </c>
-      <c r="I15" s="12">
-        <f>(E15-F15)*D15</f>
-        <v>2.04</v>
-      </c>
-      <c r="J15" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>334</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>332</v>
-      </c>
-      <c r="D16" s="1">
-        <v>0.38</v>
-      </c>
-      <c r="E16" s="7">
-        <v>2</v>
-      </c>
-      <c r="F16" s="7">
-        <v>0</v>
-      </c>
-      <c r="G16" s="1">
-        <f>F16*D16</f>
-        <v>0</v>
-      </c>
-      <c r="H16" s="12">
-        <f t="shared" si="2"/>
-        <v>0.76</v>
-      </c>
-      <c r="I16" s="12">
-        <f>(E16-F16)*D16</f>
-        <v>0.76</v>
-      </c>
-      <c r="J16" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>335</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>333</v>
-      </c>
-      <c r="D17" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="E17" s="7">
-        <v>2</v>
-      </c>
-      <c r="F17" s="7">
-        <v>0</v>
-      </c>
-      <c r="G17" s="1">
-        <f>F17*D17</f>
-        <v>0</v>
-      </c>
-      <c r="H17" s="12">
-        <f t="shared" si="2"/>
-        <v>0.8</v>
-      </c>
-      <c r="I17" s="12">
-        <f>(E17-F17)*D17</f>
-        <v>0.8</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>337</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>338</v>
-      </c>
-      <c r="D18" s="1">
-        <v>0.86</v>
-      </c>
-      <c r="E18" s="7">
-        <v>2</v>
-      </c>
-      <c r="F18" s="7">
-        <v>0</v>
-      </c>
-      <c r="G18" s="1">
-        <f>F18*D18</f>
-        <v>0</v>
-      </c>
-      <c r="H18" s="12">
-        <f t="shared" si="2"/>
-        <v>1.72</v>
-      </c>
-      <c r="I18" s="12">
-        <f>(E18-F18)*D18</f>
-        <v>1.72</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>354</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>355</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1.02</v>
-      </c>
-      <c r="E19" s="7">
-        <v>2</v>
-      </c>
-      <c r="F19" s="7">
-        <v>0</v>
-      </c>
-      <c r="G19" s="1">
-        <f>F19*D19</f>
-        <v>0</v>
-      </c>
-      <c r="H19" s="12">
-        <f t="shared" si="2"/>
-        <v>2.04</v>
-      </c>
-      <c r="I19" s="12">
-        <f>(E19-F19)*D19</f>
-        <v>2.04</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>340</v>
-      </c>
-      <c r="B20">
-        <v>16</v>
-      </c>
-      <c r="C20" t="s">
-        <v>343</v>
-      </c>
-      <c r="D20" s="1">
-        <v>0.122</v>
-      </c>
-      <c r="E20" s="7">
-        <v>100</v>
-      </c>
-      <c r="F20" s="7">
-        <v>0</v>
-      </c>
-      <c r="G20" s="1">
-        <f>F20*D20</f>
-        <v>0</v>
-      </c>
-      <c r="H20" s="12">
-        <f t="shared" si="2"/>
-        <v>12.2</v>
-      </c>
-      <c r="I20" s="12">
-        <f>(E20-F20)*D20</f>
-        <v>12.2</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>342</v>
-      </c>
-      <c r="B21">
-        <v>16</v>
-      </c>
-      <c r="C21" t="s">
-        <v>344</v>
-      </c>
-      <c r="D21" s="1">
-        <v>0.114</v>
-      </c>
-      <c r="E21" s="7">
-        <v>100</v>
-      </c>
-      <c r="F21" s="7">
-        <v>0</v>
-      </c>
-      <c r="G21" s="1">
-        <f>F21*D21</f>
-        <v>0</v>
-      </c>
-      <c r="H21" s="12">
-        <f t="shared" si="2"/>
-        <v>11.4</v>
-      </c>
-      <c r="I21" s="12">
-        <f>(E21-F21)*D21</f>
-        <v>11.4</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>356</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
-        <v>357</v>
-      </c>
-      <c r="D22" s="1">
-        <v>89.54</v>
-      </c>
-      <c r="E22" s="7">
-        <v>1</v>
-      </c>
-      <c r="F22" s="7">
-        <v>0</v>
-      </c>
-      <c r="G22" s="1">
-        <f>F22*D22</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="12">
-        <f t="shared" si="2"/>
-        <v>89.54</v>
-      </c>
-      <c r="I22" s="12">
-        <f>(E22-F22)*D22</f>
-        <v>89.54</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>352</v>
-      </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
-        <v>353</v>
-      </c>
-      <c r="D23" s="1">
-        <v>8.9</v>
-      </c>
-      <c r="E23" s="7">
-        <v>1</v>
-      </c>
-      <c r="F23" s="7">
-        <v>0</v>
-      </c>
-      <c r="G23" s="1">
-        <f>F23*D23</f>
-        <v>0</v>
-      </c>
-      <c r="H23" s="12">
-        <f t="shared" si="2"/>
-        <v>8.9</v>
-      </c>
-      <c r="I23" s="12">
-        <f>(E23-F23)*D23</f>
-        <v>8.9</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G24" s="1">
-        <f>SUM(G14:G23)</f>
-        <v>0</v>
-      </c>
-      <c r="H24" s="1">
-        <f>SUM(H14:H23)</f>
-        <v>137.70000000000002</v>
-      </c>
-      <c r="I24" s="1">
-        <f>SUM(I14:I23)</f>
-        <v>137.70000000000002</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
-        <v>376</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>363</v>
-      </c>
-      <c r="F26" s="9"/>
-      <c r="H26" s="10" t="s">
-        <v>361</v>
-      </c>
-      <c r="I26" s="11"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
-        <v>254</v>
-      </c>
-      <c r="C27" t="s">
-        <v>2</v>
-      </c>
-      <c r="D27" t="s">
-        <v>114</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>364</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>365</v>
-      </c>
-      <c r="G27" t="s">
-        <v>366</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>360</v>
-      </c>
-      <c r="I27" s="11" t="s">
-        <v>362</v>
-      </c>
-      <c r="J27" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>96</v>
-      </c>
-      <c r="B28">
-        <v>28</v>
-      </c>
-      <c r="C28" t="s">
-        <v>294</v>
-      </c>
-      <c r="D28" s="1">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="E28" s="7">
-        <v>100</v>
-      </c>
-      <c r="F28" s="7">
-        <v>0</v>
-      </c>
-      <c r="G28" s="1">
-        <f>F28*D28</f>
-        <v>0</v>
-      </c>
-      <c r="H28" s="12">
-        <f>D28*E28</f>
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="I28" s="12">
-        <f>(E28-F28)*D28</f>
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="J28" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>292</v>
-      </c>
-      <c r="B29">
-        <v>2</v>
-      </c>
-      <c r="C29" t="s">
-        <v>293</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1.02</v>
-      </c>
-      <c r="E29" s="7">
-        <v>2</v>
-      </c>
-      <c r="F29" s="7">
-        <v>0</v>
-      </c>
-      <c r="G29" s="1">
-        <f>F29*D29</f>
-        <v>0</v>
-      </c>
-      <c r="H29" s="12">
-        <f t="shared" ref="H29:H37" si="3">D29*E29</f>
-        <v>2.04</v>
-      </c>
-      <c r="I29" s="12">
-        <f>(E29-F29)*D29</f>
-        <v>2.04</v>
-      </c>
-      <c r="J29" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>334</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
-        <v>332</v>
-      </c>
-      <c r="D30" s="1">
-        <v>0.38</v>
-      </c>
-      <c r="E30" s="7">
-        <v>2</v>
-      </c>
-      <c r="F30" s="7">
-        <v>0</v>
-      </c>
-      <c r="G30" s="1">
-        <f>F30*D30</f>
-        <v>0</v>
-      </c>
-      <c r="H30" s="12">
-        <f t="shared" si="3"/>
-        <v>0.76</v>
-      </c>
-      <c r="I30" s="12">
-        <f>(E30-F30)*D30</f>
-        <v>0.76</v>
-      </c>
-      <c r="J30" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>335</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
-        <v>333</v>
-      </c>
-      <c r="D31" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="E31" s="7">
-        <v>2</v>
-      </c>
-      <c r="F31" s="7">
-        <v>0</v>
-      </c>
-      <c r="G31" s="1">
-        <f>F31*D31</f>
-        <v>0</v>
-      </c>
-      <c r="H31" s="12">
-        <f t="shared" si="3"/>
-        <v>0.8</v>
-      </c>
-      <c r="I31" s="12">
-        <f>(E31-F31)*D31</f>
-        <v>0.8</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>337</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s">
-        <v>338</v>
-      </c>
-      <c r="D32" s="1">
-        <v>0.86</v>
-      </c>
-      <c r="E32" s="7">
-        <v>2</v>
-      </c>
-      <c r="F32" s="7">
-        <v>0</v>
-      </c>
-      <c r="G32" s="1">
-        <f>F32*D32</f>
-        <v>0</v>
-      </c>
-      <c r="H32" s="12">
-        <f t="shared" si="3"/>
-        <v>1.72</v>
-      </c>
-      <c r="I32" s="12">
-        <f>(E32-F32)*D32</f>
-        <v>1.72</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>354</v>
-      </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-      <c r="C33" t="s">
-        <v>355</v>
-      </c>
-      <c r="D33" s="1">
-        <v>1.02</v>
-      </c>
-      <c r="E33" s="7">
-        <v>2</v>
-      </c>
-      <c r="F33" s="7">
-        <v>0</v>
-      </c>
-      <c r="G33" s="1">
-        <f>F33*D33</f>
-        <v>0</v>
-      </c>
-      <c r="H33" s="12">
-        <f t="shared" si="3"/>
-        <v>2.04</v>
-      </c>
-      <c r="I33" s="12">
-        <f>(E33-F33)*D33</f>
-        <v>2.04</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>340</v>
-      </c>
-      <c r="B34">
-        <v>16</v>
-      </c>
-      <c r="C34" t="s">
-        <v>343</v>
-      </c>
-      <c r="D34" s="1">
-        <v>0.122</v>
-      </c>
-      <c r="E34" s="7">
-        <v>100</v>
-      </c>
-      <c r="F34" s="7">
-        <v>0</v>
-      </c>
-      <c r="G34" s="1">
-        <f>F34*D34</f>
-        <v>0</v>
-      </c>
-      <c r="H34" s="12">
-        <f t="shared" si="3"/>
-        <v>12.2</v>
-      </c>
-      <c r="I34" s="12">
-        <f>(E34-F34)*D34</f>
-        <v>12.2</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>342</v>
-      </c>
-      <c r="B35">
-        <v>16</v>
-      </c>
-      <c r="C35" t="s">
-        <v>344</v>
-      </c>
-      <c r="D35" s="1">
-        <v>0.114</v>
-      </c>
-      <c r="E35" s="7">
-        <v>100</v>
-      </c>
-      <c r="F35" s="7">
-        <v>0</v>
-      </c>
-      <c r="G35" s="1">
-        <f>F35*D35</f>
-        <v>0</v>
-      </c>
-      <c r="H35" s="12">
-        <f t="shared" si="3"/>
-        <v>11.4</v>
-      </c>
-      <c r="I35" s="12">
-        <f>(E35-F35)*D35</f>
-        <v>11.4</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>356</v>
-      </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36" t="s">
-        <v>357</v>
-      </c>
-      <c r="D36" s="1">
-        <v>89.54</v>
-      </c>
-      <c r="E36" s="7">
-        <v>1</v>
-      </c>
-      <c r="F36" s="7">
-        <v>0</v>
-      </c>
-      <c r="G36" s="1">
-        <f>F36*D36</f>
-        <v>0</v>
-      </c>
-      <c r="H36" s="12">
-        <f t="shared" si="3"/>
-        <v>89.54</v>
-      </c>
-      <c r="I36" s="12">
-        <f>(E36-F36)*D36</f>
-        <v>89.54</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>352</v>
-      </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
-        <v>353</v>
-      </c>
-      <c r="D37" s="1">
-        <v>8.9</v>
-      </c>
-      <c r="E37" s="7">
-        <v>1</v>
-      </c>
-      <c r="F37" s="7">
-        <v>0</v>
-      </c>
-      <c r="G37" s="1">
-        <f>F37*D37</f>
-        <v>0</v>
-      </c>
-      <c r="H37" s="12">
-        <f t="shared" si="3"/>
-        <v>8.9</v>
-      </c>
-      <c r="I37" s="12">
-        <f>(E37-F37)*D37</f>
-        <v>8.9</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G38" s="1">
-        <f>SUM(G28:G37)</f>
-        <v>0</v>
-      </c>
-      <c r="H38" s="1">
-        <f>SUM(H28:H37)</f>
-        <v>137.70000000000002</v>
-      </c>
-      <c r="I38" s="1">
-        <f>SUM(I28:I37)</f>
-        <v>137.70000000000002</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>103</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="J17" r:id="rId1" xr:uid="{8F88ED9B-1C89-4651-AF81-0D0D1136F20A}"/>
-    <hyperlink ref="J31" r:id="rId2" xr:uid="{6D16E149-47DE-4D84-AA2C-CEB7B48F918E}"/>
-  </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{645409AD-79BA-4214-8D29-3BF242B131B1}">
-  <dimension ref="A1:J63"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="57.5" customWidth="1"/>
-    <col min="2" max="2" width="10.5" customWidth="1"/>
-    <col min="3" max="3" width="34.375" customWidth="1"/>
-    <col min="4" max="4" width="11.5" customWidth="1"/>
-    <col min="5" max="5" width="7.375" customWidth="1"/>
-    <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="10.375" customWidth="1"/>
-    <col min="8" max="8" width="9.875" customWidth="1"/>
-    <col min="9" max="9" width="10.375" customWidth="1"/>
-    <col min="10" max="10" width="18.125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="6" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>363</v>
-      </c>
-      <c r="F4" s="9"/>
-      <c r="H4" s="10" t="s">
-        <v>389</v>
-      </c>
-      <c r="I4" s="11"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>254</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>114</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>364</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>365</v>
-      </c>
-      <c r="G5" t="s">
-        <v>366</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>387</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>388</v>
-      </c>
-      <c r="J5" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>383</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>390</v>
-      </c>
-      <c r="D6" s="1">
-        <v>80</v>
-      </c>
-      <c r="E6" s="7">
-        <v>1</v>
-      </c>
-      <c r="F6" s="7">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1">
-        <f>F6*D6</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="12">
-        <f>D6*E6</f>
-        <v>80</v>
-      </c>
-      <c r="I6" s="12">
-        <f>(E6-F6)*D6</f>
-        <v>80</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>385</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>391</v>
-      </c>
-      <c r="D7" s="1">
-        <v>5</v>
-      </c>
-      <c r="E7" s="7">
-        <v>1</v>
-      </c>
-      <c r="F7" s="7">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1">
-        <f>F7*D7</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="12">
-        <f>D7*E7</f>
-        <v>5</v>
-      </c>
-      <c r="I7" s="12">
-        <f>(E7-F7)*D7</f>
-        <v>5</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>324</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>325</v>
-      </c>
-      <c r="D8" s="1">
-        <v>15.99</v>
-      </c>
-      <c r="E8" s="7">
-        <v>1</v>
-      </c>
-      <c r="F8" s="7">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1">
-        <f>F8*D8</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="12">
-        <f t="shared" ref="H8:H10" si="0">D8*E8</f>
-        <v>15.99</v>
-      </c>
-      <c r="I8" s="12">
-        <f>(E8-F8)*D8</f>
-        <v>15.99</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>349</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>350</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
-      <c r="E9" s="7">
-        <v>1</v>
-      </c>
-      <c r="F9" s="7">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <f>F9*D9</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="12">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I9" s="12">
-        <f>(E9-F9)*D9</f>
-        <v>1</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>359</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>392</v>
-      </c>
-      <c r="D10" s="1">
-        <v>14.36</v>
-      </c>
-      <c r="E10" s="7">
-        <v>1</v>
-      </c>
-      <c r="F10" s="7">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1">
-        <f>F10*D10</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="12">
-        <f t="shared" si="0"/>
-        <v>14.36</v>
-      </c>
-      <c r="I10" s="12">
-        <f>(E10-F10)*D10</f>
-        <v>14.36</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D11" s="1"/>
-      <c r="G11" s="1">
-        <f>SUM(G8:G10)</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="14">
-        <f>SUM(H6:H10)</f>
-        <v>116.35</v>
-      </c>
-      <c r="I11" s="1">
-        <f>SUM(I6:I10)</f>
-        <v>116.35</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>103</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="J6" r:id="rId1" display="https://www.mouser.com/ProductDetail/Raspberry-Pi/SC1112?qs=HoCaDK9Nz5c86n0i5EQ%2FPA%3D%3D" xr:uid="{1AD7AD03-BA63-4D8F-89EC-00A7DFC89138}"/>
-    <hyperlink ref="J7" r:id="rId2" display="https://www.mouser.com/ProductDetail/Raspberry-Pi/SC1148?qs=HoCaDK9Nz5fqo0izK2taew%3D%3D" xr:uid="{3B3FFB0D-A2AF-4610-B56A-77263F3DF5B7}"/>
-    <hyperlink ref="J8" r:id="rId3" xr:uid="{64585390-A70C-4A01-8458-C19F01A4A832}"/>
+    <hyperlink ref="J7" r:id="rId1" display="https://www.mouser.com/ProductDetail/Raspberry-Pi/SC1112?qs=HoCaDK9Nz5c86n0i5EQ%2FPA%3D%3D" xr:uid="{1AD7AD03-BA63-4D8F-89EC-00A7DFC89138}"/>
+    <hyperlink ref="J8" r:id="rId2" display="https://www.mouser.com/ProductDetail/Raspberry-Pi/SC1148?qs=HoCaDK9Nz5fqo0izK2taew%3D%3D" xr:uid="{3B3FFB0D-A2AF-4610-B56A-77263F3DF5B7}"/>
+    <hyperlink ref="J9" r:id="rId3" xr:uid="{64585390-A70C-4A01-8458-C19F01A4A832}"/>
+    <hyperlink ref="J16" r:id="rId4" xr:uid="{774058EF-55F5-470A-8B4B-4F904B944C1B}"/>
+    <hyperlink ref="J17" r:id="rId5" xr:uid="{B9FAFB4B-6A15-4D3B-BDFA-9B27F5A7CAF8}"/>
+    <hyperlink ref="J18" r:id="rId6" xr:uid="{30EB2E47-D6E5-4813-998C-D60BDF669467}"/>
+    <hyperlink ref="J19" r:id="rId7" xr:uid="{05862E78-9D45-4555-81BE-F14C0BBA8A39}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -3918,7 +4257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4686087C-B58C-7A42-AAAC-3D022FB0521D}">
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -3941,7 +4280,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>